<commit_message>
edit by ngy.hai 250404
</commit_message>
<xml_diff>
--- a/2025 DZ.xlsx
+++ b/2025 DZ.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10329"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nguyenhai/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HAI_NGUYEN\Desktop\TỔNG KẾT\Github-learn\knowledge-2025\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2DA0DDCC-F754-5843-BE53-63656E9A91BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95E9D0D2-568F-4F1C-9AB5-C46F57AE3036}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="30720" windowHeight="17240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="25年案" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="44">
   <si>
     <t>2025/2/1 総務部</t>
   </si>
@@ -414,12 +414,16 @@
     </r>
     <phoneticPr fontId="10"/>
   </si>
+  <si>
+    <t>Con khoang 3 tuan nua thoi!!!</t>
+    <phoneticPr fontId="10"/>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="13" x14ac:knownFonts="1">
+  <fonts count="14">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -513,6 +517,14 @@
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="MS PGothic"/>
+      <family val="3"/>
+      <charset val="128"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="7">
@@ -995,7 +1007,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="72">
+  <cellXfs count="73">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -1131,6 +1143,27 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -1140,70 +1173,52 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="55" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="55" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -1557,13 +1572,13 @@
   </sheetPr>
   <dimension ref="A1:AB1000"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A2" zoomScale="150" workbookViewId="0">
-      <selection activeCell="AA13" sqref="AA13"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="Z11" sqref="Z11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="3.5" customWidth="1"/>
+    <col min="1" max="1" width="3.44140625" customWidth="1"/>
     <col min="2" max="8" width="3.6640625" customWidth="1"/>
     <col min="9" max="9" width="1.33203125" customWidth="1"/>
     <col min="10" max="10" width="3.6640625" customWidth="1"/>
@@ -1574,46 +1589,46 @@
     <col min="26" max="28" width="8" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:28" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:28" ht="15" customHeight="1">
       <c r="X1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:28" ht="15" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="C2" s="61" t="s">
+    <row r="2" spans="1:28" ht="15" customHeight="1">
+      <c r="C2" s="71" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="62"/>
-      <c r="E2" s="62"/>
-      <c r="F2" s="62"/>
-      <c r="G2" s="62"/>
-      <c r="H2" s="62"/>
-      <c r="I2" s="62"/>
-      <c r="J2" s="62"/>
-      <c r="K2" s="62"/>
-      <c r="L2" s="62"/>
-      <c r="M2" s="62"/>
-      <c r="N2" s="62"/>
-      <c r="O2" s="62"/>
-      <c r="P2" s="62"/>
-      <c r="Q2" s="62"/>
-      <c r="R2" s="62"/>
-      <c r="S2" s="62"/>
-      <c r="T2" s="62"/>
-      <c r="U2" s="62"/>
-      <c r="V2" s="62"/>
-      <c r="W2" s="62"/>
-      <c r="X2" s="62"/>
-    </row>
-    <row r="4" spans="1:28" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="D2" s="53"/>
+      <c r="E2" s="53"/>
+      <c r="F2" s="53"/>
+      <c r="G2" s="53"/>
+      <c r="H2" s="53"/>
+      <c r="I2" s="53"/>
+      <c r="J2" s="53"/>
+      <c r="K2" s="53"/>
+      <c r="L2" s="53"/>
+      <c r="M2" s="53"/>
+      <c r="N2" s="53"/>
+      <c r="O2" s="53"/>
+      <c r="P2" s="53"/>
+      <c r="Q2" s="53"/>
+      <c r="R2" s="53"/>
+      <c r="S2" s="53"/>
+      <c r="T2" s="53"/>
+      <c r="U2" s="53"/>
+      <c r="V2" s="53"/>
+      <c r="W2" s="53"/>
+      <c r="X2" s="53"/>
+    </row>
+    <row r="4" spans="1:28" ht="14.25" customHeight="1">
       <c r="A4" s="2"/>
-      <c r="B4" s="56">
+      <c r="B4" s="66">
         <v>45748</v>
       </c>
-      <c r="C4" s="57"/>
-      <c r="D4" s="57"/>
-      <c r="E4" s="57"/>
-      <c r="F4" s="57"/>
+      <c r="C4" s="67"/>
+      <c r="D4" s="67"/>
+      <c r="E4" s="67"/>
+      <c r="F4" s="67"/>
       <c r="G4" s="3">
         <v>20</v>
       </c>
@@ -1621,13 +1636,13 @@
         <v>10</v>
       </c>
       <c r="I4" s="2"/>
-      <c r="J4" s="56">
+      <c r="J4" s="66">
         <v>45778</v>
       </c>
-      <c r="K4" s="57"/>
-      <c r="L4" s="57"/>
-      <c r="M4" s="57"/>
-      <c r="N4" s="57"/>
+      <c r="K4" s="67"/>
+      <c r="L4" s="67"/>
+      <c r="M4" s="67"/>
+      <c r="N4" s="67"/>
       <c r="O4" s="3">
         <v>18</v>
       </c>
@@ -1635,13 +1650,13 @@
         <v>13</v>
       </c>
       <c r="Q4" s="2"/>
-      <c r="R4" s="56">
+      <c r="R4" s="66">
         <v>45809</v>
       </c>
-      <c r="S4" s="57"/>
-      <c r="T4" s="57"/>
-      <c r="U4" s="57"/>
-      <c r="V4" s="57"/>
+      <c r="S4" s="67"/>
+      <c r="T4" s="67"/>
+      <c r="U4" s="67"/>
+      <c r="V4" s="67"/>
       <c r="W4" s="3">
         <v>21</v>
       </c>
@@ -1653,7 +1668,7 @@
       <c r="AA4" s="2"/>
       <c r="AB4" s="2"/>
     </row>
-    <row r="5" spans="1:28" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:28" ht="14.25" customHeight="1">
       <c r="B5" s="5" t="s">
         <v>2</v>
       </c>
@@ -1720,7 +1735,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:28" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:28" ht="14.25" customHeight="1">
       <c r="B6" s="9"/>
       <c r="C6" s="10"/>
       <c r="D6" s="10">
@@ -1775,7 +1790,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="7" spans="1:28" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:28" ht="14.25" customHeight="1">
       <c r="B7" s="9">
         <v>6</v>
       </c>
@@ -1841,11 +1856,11 @@
       <c r="X7" s="11">
         <v>14</v>
       </c>
-      <c r="Z7" s="71" t="s">
+      <c r="Z7" s="47" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="8" spans="1:28" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:28" ht="14.25" customHeight="1">
       <c r="B8" s="9">
         <v>13</v>
       </c>
@@ -1911,11 +1926,11 @@
       <c r="X8" s="11">
         <v>21</v>
       </c>
-      <c r="Z8" s="71" t="s">
+      <c r="Z8" s="47" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="9" spans="1:28" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:28" ht="14.25" customHeight="1">
       <c r="B9" s="9">
         <v>20</v>
       </c>
@@ -1982,7 +1997,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="10" spans="1:28" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:28" ht="14.25" customHeight="1">
       <c r="B10" s="9">
         <v>27</v>
       </c>
@@ -2033,121 +2048,124 @@
       <c r="W10" s="10"/>
       <c r="X10" s="11"/>
     </row>
-    <row r="11" spans="1:28" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B11" s="58" t="s">
+    <row r="11" spans="1:28" ht="14.25" customHeight="1">
+      <c r="B11" s="62" t="s">
         <v>9</v>
       </c>
-      <c r="C11" s="59"/>
-      <c r="D11" s="59"/>
-      <c r="E11" s="59"/>
-      <c r="F11" s="59"/>
-      <c r="G11" s="59"/>
-      <c r="H11" s="60"/>
+      <c r="C11" s="63"/>
+      <c r="D11" s="63"/>
+      <c r="E11" s="63"/>
+      <c r="F11" s="63"/>
+      <c r="G11" s="63"/>
+      <c r="H11" s="64"/>
       <c r="I11" s="16"/>
-      <c r="J11" s="58" t="s">
+      <c r="J11" s="62" t="s">
         <v>9</v>
       </c>
-      <c r="K11" s="59"/>
-      <c r="L11" s="59"/>
-      <c r="M11" s="59"/>
-      <c r="N11" s="59"/>
-      <c r="O11" s="59"/>
-      <c r="P11" s="60"/>
+      <c r="K11" s="63"/>
+      <c r="L11" s="63"/>
+      <c r="M11" s="63"/>
+      <c r="N11" s="63"/>
+      <c r="O11" s="63"/>
+      <c r="P11" s="64"/>
       <c r="Q11" s="16"/>
-      <c r="R11" s="58" t="s">
+      <c r="R11" s="62" t="s">
         <v>9</v>
       </c>
-      <c r="S11" s="59"/>
-      <c r="T11" s="59"/>
-      <c r="U11" s="59"/>
-      <c r="V11" s="59"/>
-      <c r="W11" s="59"/>
-      <c r="X11" s="60"/>
-    </row>
-    <row r="12" spans="1:28" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="S11" s="63"/>
+      <c r="T11" s="63"/>
+      <c r="U11" s="63"/>
+      <c r="V11" s="63"/>
+      <c r="W11" s="63"/>
+      <c r="X11" s="64"/>
+      <c r="Z11" s="72" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="12" spans="1:28" ht="14.25" customHeight="1">
       <c r="B12" s="17">
         <v>29</v>
       </c>
-      <c r="C12" s="47" t="s">
+      <c r="C12" s="54" t="s">
         <v>10</v>
       </c>
-      <c r="D12" s="48"/>
-      <c r="E12" s="48"/>
-      <c r="F12" s="48"/>
-      <c r="G12" s="48"/>
-      <c r="H12" s="49"/>
+      <c r="D12" s="55"/>
+      <c r="E12" s="55"/>
+      <c r="F12" s="55"/>
+      <c r="G12" s="55"/>
+      <c r="H12" s="56"/>
       <c r="I12" s="18"/>
       <c r="J12" s="17">
         <v>3</v>
       </c>
-      <c r="K12" s="47" t="s">
+      <c r="K12" s="54" t="s">
         <v>11</v>
       </c>
-      <c r="L12" s="48"/>
-      <c r="M12" s="48"/>
-      <c r="N12" s="48"/>
-      <c r="O12" s="48"/>
-      <c r="P12" s="49"/>
+      <c r="L12" s="55"/>
+      <c r="M12" s="55"/>
+      <c r="N12" s="55"/>
+      <c r="O12" s="55"/>
+      <c r="P12" s="56"/>
       <c r="Q12" s="18"/>
-      <c r="R12" s="63" t="s">
+      <c r="R12" s="65" t="s">
         <v>12</v>
       </c>
-      <c r="S12" s="48"/>
-      <c r="T12" s="48"/>
-      <c r="U12" s="48"/>
-      <c r="V12" s="48"/>
-      <c r="W12" s="48"/>
-      <c r="X12" s="49"/>
-    </row>
-    <row r="13" spans="1:28" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="S12" s="55"/>
+      <c r="T12" s="55"/>
+      <c r="U12" s="55"/>
+      <c r="V12" s="55"/>
+      <c r="W12" s="55"/>
+      <c r="X12" s="56"/>
+    </row>
+    <row r="13" spans="1:28" ht="15" customHeight="1">
       <c r="B13" s="19"/>
-      <c r="C13" s="50"/>
-      <c r="D13" s="48"/>
-      <c r="E13" s="48"/>
-      <c r="F13" s="48"/>
-      <c r="G13" s="48"/>
-      <c r="H13" s="49"/>
+      <c r="C13" s="68"/>
+      <c r="D13" s="55"/>
+      <c r="E13" s="55"/>
+      <c r="F13" s="55"/>
+      <c r="G13" s="55"/>
+      <c r="H13" s="56"/>
       <c r="I13" s="18"/>
       <c r="J13" s="20">
         <v>4</v>
       </c>
-      <c r="K13" s="51" t="s">
+      <c r="K13" s="57" t="s">
         <v>13</v>
       </c>
-      <c r="L13" s="52"/>
-      <c r="M13" s="52"/>
-      <c r="N13" s="52"/>
-      <c r="O13" s="52"/>
-      <c r="P13" s="53"/>
+      <c r="L13" s="58"/>
+      <c r="M13" s="58"/>
+      <c r="N13" s="58"/>
+      <c r="O13" s="58"/>
+      <c r="P13" s="59"/>
       <c r="Q13" s="18"/>
-      <c r="R13" s="64"/>
-      <c r="S13" s="48"/>
-      <c r="T13" s="48"/>
-      <c r="U13" s="48"/>
-      <c r="V13" s="48"/>
-      <c r="W13" s="48"/>
-      <c r="X13" s="49"/>
-    </row>
-    <row r="14" spans="1:28" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="R13" s="60"/>
+      <c r="S13" s="55"/>
+      <c r="T13" s="55"/>
+      <c r="U13" s="55"/>
+      <c r="V13" s="55"/>
+      <c r="W13" s="55"/>
+      <c r="X13" s="56"/>
+    </row>
+    <row r="14" spans="1:28" ht="15" customHeight="1">
       <c r="B14" s="21"/>
-      <c r="C14" s="65"/>
-      <c r="D14" s="48"/>
-      <c r="E14" s="48"/>
-      <c r="F14" s="48"/>
-      <c r="G14" s="48"/>
-      <c r="H14" s="49"/>
+      <c r="C14" s="70"/>
+      <c r="D14" s="55"/>
+      <c r="E14" s="55"/>
+      <c r="F14" s="55"/>
+      <c r="G14" s="55"/>
+      <c r="H14" s="56"/>
       <c r="I14" s="18"/>
       <c r="J14" s="22">
         <v>5</v>
       </c>
-      <c r="K14" s="51" t="s">
+      <c r="K14" s="57" t="s">
         <v>14</v>
       </c>
-      <c r="L14" s="52"/>
-      <c r="M14" s="52"/>
-      <c r="N14" s="52"/>
-      <c r="O14" s="52"/>
-      <c r="P14" s="53"/>
+      <c r="L14" s="58"/>
+      <c r="M14" s="58"/>
+      <c r="N14" s="58"/>
+      <c r="O14" s="58"/>
+      <c r="P14" s="59"/>
       <c r="Q14" s="18"/>
       <c r="R14" s="23"/>
       <c r="S14" s="24"/>
@@ -2157,36 +2175,36 @@
       <c r="W14" s="24"/>
       <c r="X14" s="25"/>
     </row>
-    <row r="15" spans="1:28" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B15" s="54"/>
-      <c r="C15" s="52"/>
-      <c r="D15" s="52"/>
-      <c r="E15" s="52"/>
-      <c r="F15" s="52"/>
-      <c r="G15" s="52"/>
-      <c r="H15" s="53"/>
+    <row r="15" spans="1:28" ht="13.5" customHeight="1">
+      <c r="B15" s="61"/>
+      <c r="C15" s="58"/>
+      <c r="D15" s="58"/>
+      <c r="E15" s="58"/>
+      <c r="F15" s="58"/>
+      <c r="G15" s="58"/>
+      <c r="H15" s="59"/>
       <c r="I15" s="26"/>
       <c r="J15" s="22">
         <v>6</v>
       </c>
-      <c r="K15" s="51" t="s">
+      <c r="K15" s="57" t="s">
         <v>15</v>
       </c>
-      <c r="L15" s="52"/>
-      <c r="M15" s="52"/>
-      <c r="N15" s="52"/>
-      <c r="O15" s="52"/>
-      <c r="P15" s="53"/>
+      <c r="L15" s="58"/>
+      <c r="M15" s="58"/>
+      <c r="N15" s="58"/>
+      <c r="O15" s="58"/>
+      <c r="P15" s="59"/>
       <c r="Q15" s="18"/>
-      <c r="R15" s="54"/>
-      <c r="S15" s="52"/>
-      <c r="T15" s="52"/>
-      <c r="U15" s="52"/>
-      <c r="V15" s="52"/>
-      <c r="W15" s="52"/>
-      <c r="X15" s="53"/>
-    </row>
-    <row r="16" spans="1:28" ht="6" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="R15" s="61"/>
+      <c r="S15" s="58"/>
+      <c r="T15" s="58"/>
+      <c r="U15" s="58"/>
+      <c r="V15" s="58"/>
+      <c r="W15" s="58"/>
+      <c r="X15" s="59"/>
+    </row>
+    <row r="16" spans="1:28" ht="6" customHeight="1">
       <c r="B16" s="26"/>
       <c r="C16" s="26"/>
       <c r="D16" s="26"/>
@@ -2211,15 +2229,15 @@
       <c r="W16" s="26"/>
       <c r="X16" s="26"/>
     </row>
-    <row r="17" spans="1:28" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:28" ht="14.25" customHeight="1">
       <c r="A17" s="2"/>
-      <c r="B17" s="56">
+      <c r="B17" s="66">
         <v>45839</v>
       </c>
-      <c r="C17" s="57"/>
-      <c r="D17" s="57"/>
-      <c r="E17" s="57"/>
-      <c r="F17" s="57"/>
+      <c r="C17" s="67"/>
+      <c r="D17" s="67"/>
+      <c r="E17" s="67"/>
+      <c r="F17" s="67"/>
       <c r="G17" s="3">
         <v>23</v>
       </c>
@@ -2227,13 +2245,13 @@
         <v>8</v>
       </c>
       <c r="I17" s="2"/>
-      <c r="J17" s="56">
+      <c r="J17" s="66">
         <v>45870</v>
       </c>
-      <c r="K17" s="57"/>
-      <c r="L17" s="57"/>
-      <c r="M17" s="57"/>
-      <c r="N17" s="57"/>
+      <c r="K17" s="67"/>
+      <c r="L17" s="67"/>
+      <c r="M17" s="67"/>
+      <c r="N17" s="67"/>
       <c r="O17" s="3">
         <v>16</v>
       </c>
@@ -2241,13 +2259,13 @@
         <v>15</v>
       </c>
       <c r="Q17" s="2"/>
-      <c r="R17" s="56">
+      <c r="R17" s="66">
         <v>45901</v>
       </c>
-      <c r="S17" s="57"/>
-      <c r="T17" s="57"/>
-      <c r="U17" s="57"/>
-      <c r="V17" s="57"/>
+      <c r="S17" s="67"/>
+      <c r="T17" s="67"/>
+      <c r="U17" s="67"/>
+      <c r="V17" s="67"/>
       <c r="W17" s="3">
         <v>22</v>
       </c>
@@ -2259,7 +2277,7 @@
       <c r="AA17" s="2"/>
       <c r="AB17" s="2"/>
     </row>
-    <row r="18" spans="1:28" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:28" ht="14.25" customHeight="1">
       <c r="B18" s="5" t="s">
         <v>2</v>
       </c>
@@ -2326,7 +2344,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="19" spans="1:28" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:28" ht="14.25" customHeight="1">
       <c r="B19" s="9"/>
       <c r="C19" s="10"/>
       <c r="D19" s="10">
@@ -2377,7 +2395,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="20" spans="1:28" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:28" ht="14.25" customHeight="1">
       <c r="B20" s="9">
         <v>6</v>
       </c>
@@ -2444,7 +2462,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="21" spans="1:28" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:28" ht="14.25" customHeight="1">
       <c r="B21" s="9">
         <v>13</v>
       </c>
@@ -2511,7 +2529,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="22" spans="1:28" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:28" ht="14.25" customHeight="1">
       <c r="B22" s="9">
         <v>20</v>
       </c>
@@ -2578,7 +2596,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="23" spans="1:28" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:28" ht="14.25" customHeight="1">
       <c r="B23" s="9">
         <v>27</v>
       </c>
@@ -2633,7 +2651,7 @@
       <c r="W23" s="10"/>
       <c r="X23" s="11"/>
     </row>
-    <row r="24" spans="1:28" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:28" ht="14.25" customHeight="1">
       <c r="B24" s="9"/>
       <c r="C24" s="10"/>
       <c r="D24" s="10"/>
@@ -2660,129 +2678,129 @@
       <c r="W24" s="10"/>
       <c r="X24" s="11"/>
     </row>
-    <row r="25" spans="1:28" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B25" s="58" t="s">
+    <row r="25" spans="1:28" ht="14.25" customHeight="1">
+      <c r="B25" s="62" t="s">
         <v>9</v>
       </c>
-      <c r="C25" s="59"/>
-      <c r="D25" s="59"/>
-      <c r="E25" s="59"/>
-      <c r="F25" s="59"/>
-      <c r="G25" s="59"/>
-      <c r="H25" s="60"/>
+      <c r="C25" s="63"/>
+      <c r="D25" s="63"/>
+      <c r="E25" s="63"/>
+      <c r="F25" s="63"/>
+      <c r="G25" s="63"/>
+      <c r="H25" s="64"/>
       <c r="I25" s="16"/>
-      <c r="J25" s="58" t="s">
+      <c r="J25" s="62" t="s">
         <v>9</v>
       </c>
-      <c r="K25" s="59"/>
-      <c r="L25" s="59"/>
-      <c r="M25" s="59"/>
-      <c r="N25" s="59"/>
-      <c r="O25" s="59"/>
-      <c r="P25" s="60"/>
+      <c r="K25" s="63"/>
+      <c r="L25" s="63"/>
+      <c r="M25" s="63"/>
+      <c r="N25" s="63"/>
+      <c r="O25" s="63"/>
+      <c r="P25" s="64"/>
       <c r="Q25" s="16"/>
-      <c r="R25" s="58" t="s">
+      <c r="R25" s="62" t="s">
         <v>9</v>
       </c>
-      <c r="S25" s="59"/>
-      <c r="T25" s="59"/>
-      <c r="U25" s="59"/>
-      <c r="V25" s="59"/>
-      <c r="W25" s="59"/>
-      <c r="X25" s="60"/>
-    </row>
-    <row r="26" spans="1:28" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="S25" s="63"/>
+      <c r="T25" s="63"/>
+      <c r="U25" s="63"/>
+      <c r="V25" s="63"/>
+      <c r="W25" s="63"/>
+      <c r="X25" s="64"/>
+    </row>
+    <row r="26" spans="1:28" ht="14.25" customHeight="1">
       <c r="B26" s="17">
         <v>21</v>
       </c>
-      <c r="C26" s="47" t="s">
+      <c r="C26" s="54" t="s">
         <v>16</v>
       </c>
-      <c r="D26" s="48"/>
-      <c r="E26" s="48"/>
-      <c r="F26" s="48"/>
-      <c r="G26" s="48"/>
-      <c r="H26" s="49"/>
+      <c r="D26" s="55"/>
+      <c r="E26" s="55"/>
+      <c r="F26" s="55"/>
+      <c r="G26" s="55"/>
+      <c r="H26" s="56"/>
       <c r="I26" s="18"/>
       <c r="J26" s="17">
         <v>11</v>
       </c>
-      <c r="K26" s="47" t="s">
+      <c r="K26" s="54" t="s">
         <v>17</v>
       </c>
-      <c r="L26" s="48"/>
-      <c r="M26" s="48"/>
-      <c r="N26" s="48"/>
-      <c r="O26" s="48"/>
-      <c r="P26" s="49"/>
+      <c r="L26" s="55"/>
+      <c r="M26" s="55"/>
+      <c r="N26" s="55"/>
+      <c r="O26" s="55"/>
+      <c r="P26" s="56"/>
       <c r="Q26" s="18"/>
       <c r="R26" s="17">
         <v>15</v>
       </c>
-      <c r="S26" s="47" t="s">
+      <c r="S26" s="54" t="s">
         <v>18</v>
       </c>
-      <c r="T26" s="48"/>
-      <c r="U26" s="48"/>
-      <c r="V26" s="48"/>
-      <c r="W26" s="48"/>
-      <c r="X26" s="49"/>
-    </row>
-    <row r="27" spans="1:28" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="T26" s="55"/>
+      <c r="U26" s="55"/>
+      <c r="V26" s="55"/>
+      <c r="W26" s="55"/>
+      <c r="X26" s="56"/>
+    </row>
+    <row r="27" spans="1:28" ht="14.25" customHeight="1">
       <c r="B27" s="21"/>
-      <c r="C27" s="50"/>
-      <c r="D27" s="48"/>
-      <c r="E27" s="48"/>
-      <c r="F27" s="48"/>
-      <c r="G27" s="48"/>
-      <c r="H27" s="49"/>
+      <c r="C27" s="68"/>
+      <c r="D27" s="55"/>
+      <c r="E27" s="55"/>
+      <c r="F27" s="55"/>
+      <c r="G27" s="55"/>
+      <c r="H27" s="56"/>
       <c r="I27" s="18"/>
-      <c r="J27" s="54"/>
-      <c r="K27" s="52"/>
-      <c r="L27" s="52"/>
-      <c r="M27" s="52"/>
-      <c r="N27" s="52"/>
-      <c r="O27" s="52"/>
-      <c r="P27" s="53"/>
+      <c r="J27" s="61"/>
+      <c r="K27" s="58"/>
+      <c r="L27" s="58"/>
+      <c r="M27" s="58"/>
+      <c r="N27" s="58"/>
+      <c r="O27" s="58"/>
+      <c r="P27" s="59"/>
       <c r="Q27" s="18"/>
       <c r="R27" s="20">
         <v>23</v>
       </c>
-      <c r="S27" s="51" t="s">
+      <c r="S27" s="57" t="s">
         <v>19</v>
       </c>
-      <c r="T27" s="52"/>
-      <c r="U27" s="52"/>
-      <c r="V27" s="52"/>
-      <c r="W27" s="52"/>
-      <c r="X27" s="53"/>
-    </row>
-    <row r="28" spans="1:28" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="T27" s="58"/>
+      <c r="U27" s="58"/>
+      <c r="V27" s="58"/>
+      <c r="W27" s="58"/>
+      <c r="X27" s="59"/>
+    </row>
+    <row r="28" spans="1:28" ht="13.5" customHeight="1">
       <c r="B28" s="30"/>
-      <c r="C28" s="55"/>
-      <c r="D28" s="52"/>
-      <c r="E28" s="52"/>
-      <c r="F28" s="52"/>
-      <c r="G28" s="52"/>
-      <c r="H28" s="53"/>
+      <c r="C28" s="69"/>
+      <c r="D28" s="58"/>
+      <c r="E28" s="58"/>
+      <c r="F28" s="58"/>
+      <c r="G28" s="58"/>
+      <c r="H28" s="59"/>
       <c r="I28" s="26"/>
       <c r="J28" s="30"/>
-      <c r="K28" s="55"/>
-      <c r="L28" s="52"/>
-      <c r="M28" s="52"/>
-      <c r="N28" s="52"/>
-      <c r="O28" s="52"/>
-      <c r="P28" s="53"/>
+      <c r="K28" s="69"/>
+      <c r="L28" s="58"/>
+      <c r="M28" s="58"/>
+      <c r="N28" s="58"/>
+      <c r="O28" s="58"/>
+      <c r="P28" s="59"/>
       <c r="Q28" s="26"/>
-      <c r="R28" s="54"/>
-      <c r="S28" s="52"/>
-      <c r="T28" s="52"/>
-      <c r="U28" s="52"/>
-      <c r="V28" s="52"/>
-      <c r="W28" s="52"/>
-      <c r="X28" s="53"/>
-    </row>
-    <row r="29" spans="1:28" ht="6" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="R28" s="61"/>
+      <c r="S28" s="58"/>
+      <c r="T28" s="58"/>
+      <c r="U28" s="58"/>
+      <c r="V28" s="58"/>
+      <c r="W28" s="58"/>
+      <c r="X28" s="59"/>
+    </row>
+    <row r="29" spans="1:28" ht="6" customHeight="1">
       <c r="B29" s="26"/>
       <c r="C29" s="26"/>
       <c r="D29" s="26"/>
@@ -2807,15 +2825,15 @@
       <c r="W29" s="18"/>
       <c r="X29" s="18"/>
     </row>
-    <row r="30" spans="1:28" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="30" spans="1:28" ht="14.25" customHeight="1">
       <c r="A30" s="2"/>
-      <c r="B30" s="56">
+      <c r="B30" s="66">
         <v>45931</v>
       </c>
-      <c r="C30" s="57"/>
-      <c r="D30" s="57"/>
-      <c r="E30" s="57"/>
-      <c r="F30" s="57"/>
+      <c r="C30" s="67"/>
+      <c r="D30" s="67"/>
+      <c r="E30" s="67"/>
+      <c r="F30" s="67"/>
       <c r="G30" s="3">
         <v>23</v>
       </c>
@@ -2823,13 +2841,13 @@
         <v>8</v>
       </c>
       <c r="I30" s="2"/>
-      <c r="J30" s="56">
+      <c r="J30" s="66">
         <v>45962</v>
       </c>
-      <c r="K30" s="57"/>
-      <c r="L30" s="57"/>
-      <c r="M30" s="57"/>
-      <c r="N30" s="57"/>
+      <c r="K30" s="67"/>
+      <c r="L30" s="67"/>
+      <c r="M30" s="67"/>
+      <c r="N30" s="67"/>
       <c r="O30" s="3">
         <v>20</v>
       </c>
@@ -2837,13 +2855,13 @@
         <v>10</v>
       </c>
       <c r="Q30" s="2"/>
-      <c r="R30" s="56">
+      <c r="R30" s="66">
         <v>45992</v>
       </c>
-      <c r="S30" s="57"/>
-      <c r="T30" s="57"/>
-      <c r="U30" s="57"/>
-      <c r="V30" s="57"/>
+      <c r="S30" s="67"/>
+      <c r="T30" s="67"/>
+      <c r="U30" s="67"/>
+      <c r="V30" s="67"/>
       <c r="W30" s="3">
         <v>20</v>
       </c>
@@ -2855,7 +2873,7 @@
       <c r="AA30" s="2"/>
       <c r="AB30" s="2"/>
     </row>
-    <row r="31" spans="1:28" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="31" spans="1:28" ht="14.25" customHeight="1">
       <c r="B31" s="5" t="s">
         <v>2</v>
       </c>
@@ -2922,7 +2940,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="32" spans="1:28" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="32" spans="1:28" ht="14.25" customHeight="1">
       <c r="B32" s="9"/>
       <c r="C32" s="10"/>
       <c r="D32" s="10"/>
@@ -2969,7 +2987,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="33" spans="1:28" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="33" spans="1:28" ht="14.25" customHeight="1">
       <c r="B33" s="9">
         <v>5</v>
       </c>
@@ -3036,7 +3054,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="34" spans="1:28" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="34" spans="1:28" ht="14.25" customHeight="1">
       <c r="B34" s="9">
         <v>12</v>
       </c>
@@ -3103,7 +3121,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="35" spans="1:28" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="35" spans="1:28" ht="15" customHeight="1">
       <c r="B35" s="9">
         <v>19</v>
       </c>
@@ -3170,7 +3188,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="36" spans="1:28" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="36" spans="1:28" ht="15" customHeight="1">
       <c r="B36" s="31">
         <v>26</v>
       </c>
@@ -3229,7 +3247,7 @@
       <c r="W36" s="32"/>
       <c r="X36" s="33"/>
     </row>
-    <row r="37" spans="1:28" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="37" spans="1:28" ht="14.25" customHeight="1">
       <c r="B37" s="9"/>
       <c r="C37" s="10"/>
       <c r="D37" s="10"/>
@@ -3256,92 +3274,92 @@
       <c r="W37" s="10"/>
       <c r="X37" s="11"/>
     </row>
-    <row r="38" spans="1:28" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B38" s="58" t="s">
+    <row r="38" spans="1:28" ht="14.25" customHeight="1">
+      <c r="B38" s="62" t="s">
         <v>9</v>
       </c>
-      <c r="C38" s="59"/>
-      <c r="D38" s="59"/>
-      <c r="E38" s="59"/>
-      <c r="F38" s="59"/>
-      <c r="G38" s="59"/>
-      <c r="H38" s="60"/>
+      <c r="C38" s="63"/>
+      <c r="D38" s="63"/>
+      <c r="E38" s="63"/>
+      <c r="F38" s="63"/>
+      <c r="G38" s="63"/>
+      <c r="H38" s="64"/>
       <c r="I38" s="16"/>
-      <c r="J38" s="58" t="s">
+      <c r="J38" s="62" t="s">
         <v>9</v>
       </c>
-      <c r="K38" s="59"/>
-      <c r="L38" s="59"/>
-      <c r="M38" s="59"/>
-      <c r="N38" s="59"/>
-      <c r="O38" s="59"/>
-      <c r="P38" s="60"/>
+      <c r="K38" s="63"/>
+      <c r="L38" s="63"/>
+      <c r="M38" s="63"/>
+      <c r="N38" s="63"/>
+      <c r="O38" s="63"/>
+      <c r="P38" s="64"/>
       <c r="Q38" s="16"/>
-      <c r="R38" s="58" t="s">
+      <c r="R38" s="62" t="s">
         <v>9</v>
       </c>
-      <c r="S38" s="59"/>
-      <c r="T38" s="59"/>
-      <c r="U38" s="59"/>
-      <c r="V38" s="59"/>
-      <c r="W38" s="59"/>
-      <c r="X38" s="60"/>
-    </row>
-    <row r="39" spans="1:28" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="S38" s="63"/>
+      <c r="T38" s="63"/>
+      <c r="U38" s="63"/>
+      <c r="V38" s="63"/>
+      <c r="W38" s="63"/>
+      <c r="X38" s="64"/>
+    </row>
+    <row r="39" spans="1:28" ht="14.25" customHeight="1">
       <c r="B39" s="17">
         <v>13</v>
       </c>
-      <c r="C39" s="47" t="s">
+      <c r="C39" s="54" t="s">
         <v>20</v>
       </c>
-      <c r="D39" s="48"/>
-      <c r="E39" s="48"/>
-      <c r="F39" s="48"/>
-      <c r="G39" s="48"/>
-      <c r="H39" s="49"/>
+      <c r="D39" s="55"/>
+      <c r="E39" s="55"/>
+      <c r="F39" s="55"/>
+      <c r="G39" s="55"/>
+      <c r="H39" s="56"/>
       <c r="I39" s="18"/>
       <c r="J39" s="17">
         <v>3</v>
       </c>
-      <c r="K39" s="47" t="s">
+      <c r="K39" s="54" t="s">
         <v>21</v>
       </c>
-      <c r="L39" s="48"/>
-      <c r="M39" s="48"/>
-      <c r="N39" s="48"/>
-      <c r="O39" s="48"/>
-      <c r="P39" s="49"/>
+      <c r="L39" s="55"/>
+      <c r="M39" s="55"/>
+      <c r="N39" s="55"/>
+      <c r="O39" s="55"/>
+      <c r="P39" s="56"/>
       <c r="Q39" s="18"/>
-      <c r="R39" s="63" t="s">
+      <c r="R39" s="65" t="s">
         <v>12</v>
       </c>
-      <c r="S39" s="48"/>
-      <c r="T39" s="48"/>
-      <c r="U39" s="48"/>
-      <c r="V39" s="48"/>
-      <c r="W39" s="48"/>
-      <c r="X39" s="49"/>
-    </row>
-    <row r="40" spans="1:28" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="S39" s="55"/>
+      <c r="T39" s="55"/>
+      <c r="U39" s="55"/>
+      <c r="V39" s="55"/>
+      <c r="W39" s="55"/>
+      <c r="X39" s="56"/>
+    </row>
+    <row r="40" spans="1:28" ht="14.25" customHeight="1">
       <c r="B40" s="21"/>
-      <c r="C40" s="50"/>
-      <c r="D40" s="48"/>
-      <c r="E40" s="48"/>
-      <c r="F40" s="48"/>
-      <c r="G40" s="48"/>
-      <c r="H40" s="49"/>
+      <c r="C40" s="68"/>
+      <c r="D40" s="55"/>
+      <c r="E40" s="55"/>
+      <c r="F40" s="55"/>
+      <c r="G40" s="55"/>
+      <c r="H40" s="56"/>
       <c r="I40" s="18"/>
       <c r="J40" s="22">
         <v>24</v>
       </c>
-      <c r="K40" s="51" t="s">
+      <c r="K40" s="57" t="s">
         <v>22</v>
       </c>
-      <c r="L40" s="52"/>
-      <c r="M40" s="52"/>
-      <c r="N40" s="52"/>
-      <c r="O40" s="52"/>
-      <c r="P40" s="53"/>
+      <c r="L40" s="58"/>
+      <c r="M40" s="58"/>
+      <c r="N40" s="58"/>
+      <c r="O40" s="58"/>
+      <c r="P40" s="59"/>
       <c r="Q40" s="18"/>
       <c r="R40" s="35"/>
       <c r="S40" s="36"/>
@@ -3351,32 +3369,32 @@
       <c r="W40" s="36"/>
       <c r="X40" s="37"/>
     </row>
-    <row r="41" spans="1:28" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B41" s="54"/>
-      <c r="C41" s="52"/>
-      <c r="D41" s="52"/>
-      <c r="E41" s="52"/>
-      <c r="F41" s="52"/>
-      <c r="G41" s="52"/>
-      <c r="H41" s="53"/>
+    <row r="41" spans="1:28" ht="13.5" customHeight="1">
+      <c r="B41" s="61"/>
+      <c r="C41" s="58"/>
+      <c r="D41" s="58"/>
+      <c r="E41" s="58"/>
+      <c r="F41" s="58"/>
+      <c r="G41" s="58"/>
+      <c r="H41" s="59"/>
       <c r="I41" s="26"/>
-      <c r="J41" s="54"/>
-      <c r="K41" s="52"/>
-      <c r="L41" s="52"/>
-      <c r="M41" s="52"/>
-      <c r="N41" s="52"/>
-      <c r="O41" s="52"/>
-      <c r="P41" s="53"/>
+      <c r="J41" s="61"/>
+      <c r="K41" s="58"/>
+      <c r="L41" s="58"/>
+      <c r="M41" s="58"/>
+      <c r="N41" s="58"/>
+      <c r="O41" s="58"/>
+      <c r="P41" s="59"/>
       <c r="Q41" s="18"/>
       <c r="R41" s="30"/>
-      <c r="S41" s="55"/>
-      <c r="T41" s="52"/>
-      <c r="U41" s="52"/>
-      <c r="V41" s="52"/>
-      <c r="W41" s="52"/>
-      <c r="X41" s="53"/>
-    </row>
-    <row r="42" spans="1:28" ht="6" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="S41" s="69"/>
+      <c r="T41" s="58"/>
+      <c r="U41" s="58"/>
+      <c r="V41" s="58"/>
+      <c r="W41" s="58"/>
+      <c r="X41" s="59"/>
+    </row>
+    <row r="42" spans="1:28" ht="6" customHeight="1">
       <c r="B42" s="26"/>
       <c r="C42" s="26"/>
       <c r="D42" s="26"/>
@@ -3401,15 +3419,15 @@
       <c r="W42" s="18"/>
       <c r="X42" s="18"/>
     </row>
-    <row r="43" spans="1:28" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="43" spans="1:28" ht="14.25" customHeight="1">
       <c r="A43" s="2"/>
-      <c r="B43" s="56">
+      <c r="B43" s="66">
         <v>46023</v>
       </c>
-      <c r="C43" s="57"/>
-      <c r="D43" s="57"/>
-      <c r="E43" s="57"/>
-      <c r="F43" s="57"/>
+      <c r="C43" s="67"/>
+      <c r="D43" s="67"/>
+      <c r="E43" s="67"/>
+      <c r="F43" s="67"/>
       <c r="G43" s="3">
         <v>19</v>
       </c>
@@ -3417,13 +3435,13 @@
         <v>12</v>
       </c>
       <c r="I43" s="2"/>
-      <c r="J43" s="56">
+      <c r="J43" s="66">
         <v>46054</v>
       </c>
-      <c r="K43" s="57"/>
-      <c r="L43" s="57"/>
-      <c r="M43" s="57"/>
-      <c r="N43" s="57"/>
+      <c r="K43" s="67"/>
+      <c r="L43" s="67"/>
+      <c r="M43" s="67"/>
+      <c r="N43" s="67"/>
       <c r="O43" s="3">
         <v>20</v>
       </c>
@@ -3431,13 +3449,13 @@
         <v>8</v>
       </c>
       <c r="Q43" s="2"/>
-      <c r="R43" s="56">
+      <c r="R43" s="66">
         <v>46082</v>
       </c>
-      <c r="S43" s="57"/>
-      <c r="T43" s="57"/>
-      <c r="U43" s="57"/>
-      <c r="V43" s="57"/>
+      <c r="S43" s="67"/>
+      <c r="T43" s="67"/>
+      <c r="U43" s="67"/>
+      <c r="V43" s="67"/>
       <c r="W43" s="3">
         <v>22</v>
       </c>
@@ -3449,7 +3467,7 @@
       <c r="AA43" s="2"/>
       <c r="AB43" s="2"/>
     </row>
-    <row r="44" spans="1:28" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="44" spans="1:28" ht="14.25" customHeight="1">
       <c r="B44" s="5" t="s">
         <v>2</v>
       </c>
@@ -3516,7 +3534,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="45" spans="1:28" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="45" spans="1:28" ht="14.25" customHeight="1">
       <c r="B45" s="9"/>
       <c r="C45" s="10"/>
       <c r="D45" s="10"/>
@@ -3575,7 +3593,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="46" spans="1:28" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="46" spans="1:28" ht="14.25" customHeight="1">
       <c r="B46" s="9">
         <v>4</v>
       </c>
@@ -3642,7 +3660,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="47" spans="1:28" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="47" spans="1:28" ht="14.25" customHeight="1">
       <c r="B47" s="9">
         <v>11</v>
       </c>
@@ -3709,7 +3727,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="48" spans="1:28" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="48" spans="1:28" ht="14.25" customHeight="1">
       <c r="B48" s="9">
         <v>18</v>
       </c>
@@ -3776,7 +3794,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="49" spans="2:28" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="49" spans="2:28" ht="14.25" customHeight="1">
       <c r="B49" s="9">
         <v>25</v>
       </c>
@@ -3821,133 +3839,133 @@
       <c r="W49" s="10"/>
       <c r="X49" s="11"/>
     </row>
-    <row r="50" spans="2:28" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B50" s="58" t="s">
+    <row r="50" spans="2:28" ht="13.5" customHeight="1">
+      <c r="B50" s="62" t="s">
         <v>9</v>
       </c>
-      <c r="C50" s="59"/>
-      <c r="D50" s="59"/>
-      <c r="E50" s="59"/>
-      <c r="F50" s="59"/>
-      <c r="G50" s="59"/>
-      <c r="H50" s="60"/>
+      <c r="C50" s="63"/>
+      <c r="D50" s="63"/>
+      <c r="E50" s="63"/>
+      <c r="F50" s="63"/>
+      <c r="G50" s="63"/>
+      <c r="H50" s="64"/>
       <c r="I50" s="16"/>
-      <c r="J50" s="58" t="s">
+      <c r="J50" s="62" t="s">
         <v>9</v>
       </c>
-      <c r="K50" s="59"/>
-      <c r="L50" s="59"/>
-      <c r="M50" s="59"/>
-      <c r="N50" s="59"/>
-      <c r="O50" s="59"/>
-      <c r="P50" s="60"/>
+      <c r="K50" s="63"/>
+      <c r="L50" s="63"/>
+      <c r="M50" s="63"/>
+      <c r="N50" s="63"/>
+      <c r="O50" s="63"/>
+      <c r="P50" s="64"/>
       <c r="Q50" s="16"/>
-      <c r="R50" s="58" t="s">
+      <c r="R50" s="62" t="s">
         <v>9</v>
       </c>
-      <c r="S50" s="59"/>
-      <c r="T50" s="59"/>
-      <c r="U50" s="59"/>
-      <c r="V50" s="59"/>
-      <c r="W50" s="59"/>
-      <c r="X50" s="60"/>
-    </row>
-    <row r="51" spans="2:28" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="S50" s="63"/>
+      <c r="T50" s="63"/>
+      <c r="U50" s="63"/>
+      <c r="V50" s="63"/>
+      <c r="W50" s="63"/>
+      <c r="X50" s="64"/>
+    </row>
+    <row r="51" spans="2:28" ht="13.5" customHeight="1">
       <c r="B51" s="17">
         <v>1</v>
       </c>
-      <c r="C51" s="47" t="s">
+      <c r="C51" s="54" t="s">
         <v>23</v>
       </c>
-      <c r="D51" s="48"/>
-      <c r="E51" s="48"/>
-      <c r="F51" s="48"/>
-      <c r="G51" s="48"/>
-      <c r="H51" s="49"/>
+      <c r="D51" s="55"/>
+      <c r="E51" s="55"/>
+      <c r="F51" s="55"/>
+      <c r="G51" s="55"/>
+      <c r="H51" s="56"/>
       <c r="I51" s="18"/>
       <c r="J51" s="17">
         <v>11</v>
       </c>
-      <c r="K51" s="47" t="s">
+      <c r="K51" s="54" t="s">
         <v>24</v>
       </c>
-      <c r="L51" s="48"/>
-      <c r="M51" s="48"/>
-      <c r="N51" s="48"/>
-      <c r="O51" s="48"/>
-      <c r="P51" s="49"/>
+      <c r="L51" s="55"/>
+      <c r="M51" s="55"/>
+      <c r="N51" s="55"/>
+      <c r="O51" s="55"/>
+      <c r="P51" s="56"/>
       <c r="Q51" s="18"/>
       <c r="R51" s="17">
         <v>20</v>
       </c>
-      <c r="S51" s="47" t="s">
+      <c r="S51" s="54" t="s">
         <v>25</v>
       </c>
-      <c r="T51" s="48"/>
-      <c r="U51" s="48"/>
-      <c r="V51" s="48"/>
-      <c r="W51" s="48"/>
-      <c r="X51" s="49"/>
-    </row>
-    <row r="52" spans="2:28" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="T51" s="55"/>
+      <c r="U51" s="55"/>
+      <c r="V51" s="55"/>
+      <c r="W51" s="55"/>
+      <c r="X51" s="56"/>
+    </row>
+    <row r="52" spans="2:28" ht="14.25" customHeight="1">
       <c r="B52" s="22">
         <v>12</v>
       </c>
-      <c r="C52" s="51" t="s">
+      <c r="C52" s="57" t="s">
         <v>26</v>
       </c>
-      <c r="D52" s="52"/>
-      <c r="E52" s="52"/>
-      <c r="F52" s="52"/>
-      <c r="G52" s="52"/>
-      <c r="H52" s="53"/>
+      <c r="D52" s="58"/>
+      <c r="E52" s="58"/>
+      <c r="F52" s="58"/>
+      <c r="G52" s="58"/>
+      <c r="H52" s="59"/>
       <c r="I52" s="18"/>
       <c r="J52" s="17">
         <v>23</v>
       </c>
-      <c r="K52" s="47" t="s">
+      <c r="K52" s="54" t="s">
         <v>27</v>
       </c>
-      <c r="L52" s="48"/>
-      <c r="M52" s="48"/>
-      <c r="N52" s="48"/>
-      <c r="O52" s="48"/>
-      <c r="P52" s="49"/>
+      <c r="L52" s="55"/>
+      <c r="M52" s="55"/>
+      <c r="N52" s="55"/>
+      <c r="O52" s="55"/>
+      <c r="P52" s="56"/>
       <c r="Q52" s="18"/>
-      <c r="R52" s="64"/>
-      <c r="S52" s="48"/>
-      <c r="T52" s="48"/>
-      <c r="U52" s="48"/>
-      <c r="V52" s="48"/>
-      <c r="W52" s="48"/>
-      <c r="X52" s="49"/>
-    </row>
-    <row r="53" spans="2:28" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B53" s="54"/>
-      <c r="C53" s="52"/>
-      <c r="D53" s="52"/>
-      <c r="E53" s="52"/>
-      <c r="F53" s="52"/>
-      <c r="G53" s="52"/>
-      <c r="H53" s="53"/>
+      <c r="R52" s="60"/>
+      <c r="S52" s="55"/>
+      <c r="T52" s="55"/>
+      <c r="U52" s="55"/>
+      <c r="V52" s="55"/>
+      <c r="W52" s="55"/>
+      <c r="X52" s="56"/>
+    </row>
+    <row r="53" spans="2:28" ht="13.5" customHeight="1">
+      <c r="B53" s="61"/>
+      <c r="C53" s="58"/>
+      <c r="D53" s="58"/>
+      <c r="E53" s="58"/>
+      <c r="F53" s="58"/>
+      <c r="G53" s="58"/>
+      <c r="H53" s="59"/>
       <c r="I53" s="18"/>
-      <c r="J53" s="54"/>
-      <c r="K53" s="52"/>
-      <c r="L53" s="52"/>
-      <c r="M53" s="52"/>
-      <c r="N53" s="52"/>
-      <c r="O53" s="52"/>
-      <c r="P53" s="53"/>
+      <c r="J53" s="61"/>
+      <c r="K53" s="58"/>
+      <c r="L53" s="58"/>
+      <c r="M53" s="58"/>
+      <c r="N53" s="58"/>
+      <c r="O53" s="58"/>
+      <c r="P53" s="59"/>
       <c r="Q53" s="26"/>
-      <c r="R53" s="54"/>
-      <c r="S53" s="52"/>
-      <c r="T53" s="52"/>
-      <c r="U53" s="52"/>
-      <c r="V53" s="52"/>
-      <c r="W53" s="52"/>
-      <c r="X53" s="53"/>
-    </row>
-    <row r="54" spans="2:28" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="R53" s="61"/>
+      <c r="S53" s="58"/>
+      <c r="T53" s="58"/>
+      <c r="U53" s="58"/>
+      <c r="V53" s="58"/>
+      <c r="W53" s="58"/>
+      <c r="X53" s="59"/>
+    </row>
+    <row r="54" spans="2:28" ht="13.5" customHeight="1">
       <c r="Z54" s="38" t="s">
         <v>28</v>
       </c>
@@ -3955,7 +3973,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="55" spans="2:28" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="55" spans="2:28" ht="13.5" customHeight="1">
       <c r="B55" s="39"/>
       <c r="C55" s="40" t="s">
         <v>30</v>
@@ -3990,7 +4008,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="56" spans="2:28" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="56" spans="2:28" ht="13.5" customHeight="1">
       <c r="C56" s="41"/>
       <c r="D56" s="43"/>
       <c r="E56" s="43"/>
@@ -4029,7 +4047,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="57" spans="2:28" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="57" spans="2:28" ht="13.5" customHeight="1">
       <c r="B57" s="45"/>
       <c r="C57" s="40" t="s">
         <v>37</v>
@@ -4043,11 +4061,11 @@
       <c r="S57" s="43"/>
       <c r="T57" s="43"/>
       <c r="U57" s="43"/>
-      <c r="V57" s="66" t="s">
+      <c r="V57" s="48" t="s">
         <v>38</v>
       </c>
-      <c r="W57" s="67"/>
-      <c r="X57" s="68"/>
+      <c r="W57" s="49"/>
+      <c r="X57" s="50"/>
       <c r="Z57" s="38" t="s">
         <v>39</v>
       </c>
@@ -4055,7 +4073,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="58" spans="2:28" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="58" spans="2:28" ht="13.5" customHeight="1">
       <c r="B58" s="41"/>
       <c r="C58" s="41"/>
       <c r="N58" s="43"/>
@@ -4066,11 +4084,11 @@
       <c r="S58" s="43"/>
       <c r="T58" s="43"/>
       <c r="U58" s="43"/>
-      <c r="V58" s="69">
+      <c r="V58" s="51">
         <v>0</v>
       </c>
-      <c r="W58" s="67"/>
-      <c r="X58" s="68"/>
+      <c r="W58" s="49"/>
+      <c r="X58" s="50"/>
       <c r="Z58" s="38" t="s">
         <v>40</v>
       </c>
@@ -4078,21 +4096,21 @@
         <v>35</v>
       </c>
     </row>
-    <row r="59" spans="2:28" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="59" spans="2:28" ht="13.5" customHeight="1">
       <c r="B59" s="46"/>
       <c r="C59" s="41"/>
-      <c r="O59" s="70"/>
-      <c r="P59" s="62"/>
-      <c r="Q59" s="62"/>
-      <c r="R59" s="62"/>
-      <c r="S59" s="62"/>
-      <c r="T59" s="62"/>
-      <c r="U59" s="62"/>
-      <c r="V59" s="62"/>
-      <c r="W59" s="62"/>
-      <c r="X59" s="62"/>
-    </row>
-    <row r="60" spans="2:28" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="O59" s="52"/>
+      <c r="P59" s="53"/>
+      <c r="Q59" s="53"/>
+      <c r="R59" s="53"/>
+      <c r="S59" s="53"/>
+      <c r="T59" s="53"/>
+      <c r="U59" s="53"/>
+      <c r="V59" s="53"/>
+      <c r="W59" s="53"/>
+      <c r="X59" s="53"/>
+    </row>
+    <row r="60" spans="2:28" ht="13.5" customHeight="1">
       <c r="B60" s="46"/>
       <c r="C60" s="41"/>
       <c r="D60" s="41"/>
@@ -4116,7 +4134,7 @@
       <c r="V60" s="41"/>
       <c r="W60" s="41"/>
     </row>
-    <row r="61" spans="2:28" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="61" spans="2:28" ht="13.5" customHeight="1">
       <c r="B61" s="41"/>
       <c r="C61" s="41"/>
       <c r="D61" s="41"/>
@@ -4140,7 +4158,7 @@
       <c r="V61" s="41"/>
       <c r="W61" s="41"/>
     </row>
-    <row r="62" spans="2:28" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="62" spans="2:28" ht="13.5" customHeight="1">
       <c r="B62" s="41"/>
       <c r="C62" s="41"/>
       <c r="D62" s="41"/>
@@ -4164,7 +4182,7 @@
       <c r="V62" s="41"/>
       <c r="W62" s="41"/>
     </row>
-    <row r="63" spans="2:28" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="63" spans="2:28" ht="13.5" customHeight="1">
       <c r="B63" s="41"/>
       <c r="C63" s="41"/>
       <c r="D63" s="41"/>
@@ -4188,7 +4206,7 @@
       <c r="V63" s="41"/>
       <c r="W63" s="41"/>
     </row>
-    <row r="64" spans="2:28" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="64" spans="2:28" ht="13.5" customHeight="1">
       <c r="B64" s="41"/>
       <c r="C64" s="41"/>
       <c r="D64" s="41"/>
@@ -4212,7 +4230,7 @@
       <c r="V64" s="41"/>
       <c r="W64" s="41"/>
     </row>
-    <row r="65" spans="2:23" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="65" spans="2:23" ht="13.5" customHeight="1">
       <c r="B65" s="41"/>
       <c r="C65" s="41"/>
       <c r="D65" s="41"/>
@@ -4236,7 +4254,7 @@
       <c r="V65" s="41"/>
       <c r="W65" s="41"/>
     </row>
-    <row r="66" spans="2:23" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="66" spans="2:23" ht="13.5" customHeight="1">
       <c r="D66" s="41"/>
       <c r="E66" s="41"/>
       <c r="F66" s="41"/>
@@ -4258,7 +4276,7 @@
       <c r="V66" s="41"/>
       <c r="W66" s="41"/>
     </row>
-    <row r="67" spans="2:23" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="67" spans="2:23" ht="13.5" customHeight="1">
       <c r="D67" s="41"/>
       <c r="E67" s="41"/>
       <c r="F67" s="41"/>
@@ -4280,956 +4298,975 @@
       <c r="V67" s="41"/>
       <c r="W67" s="41"/>
     </row>
-    <row r="68" spans="2:23" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="69" spans="2:23" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="70" spans="2:23" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="71" spans="2:23" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="72" spans="2:23" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="73" spans="2:23" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="74" spans="2:23" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="75" spans="2:23" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="76" spans="2:23" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="77" spans="2:23" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="78" spans="2:23" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="79" spans="2:23" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="80" spans="2:23" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="81" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="82" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="83" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="84" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="85" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="86" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="87" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="88" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="89" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="90" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="91" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="92" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="93" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="94" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="95" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="96" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="97" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="98" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="99" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="100" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="101" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="102" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="103" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="104" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="105" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="106" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="107" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="108" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="109" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="110" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="111" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="112" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="113" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="114" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="115" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="116" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="117" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="118" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="119" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="120" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="121" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="122" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="123" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="124" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="125" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="126" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="127" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="128" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="129" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="130" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="131" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="132" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="133" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="134" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="135" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="136" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="137" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="138" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="139" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="140" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="141" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="142" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="143" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="144" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="145" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="146" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="147" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="148" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="149" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="150" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="151" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="152" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="153" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="154" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="155" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="156" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="157" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="158" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="159" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="160" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="161" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="162" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="163" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="164" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="165" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="166" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="167" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="168" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="169" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="170" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="171" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="172" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="173" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="174" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="175" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="176" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="177" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="178" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="179" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="180" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="181" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="182" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="183" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="184" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="185" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="186" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="187" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="188" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="189" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="190" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="191" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="192" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="193" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="194" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="195" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="196" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="197" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="198" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="199" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="200" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="201" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="202" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="203" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="204" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="205" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="206" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="207" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="208" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="209" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="210" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="211" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="212" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="213" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="214" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="215" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="216" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="217" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="218" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="219" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="220" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="221" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="222" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="223" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="224" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="225" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="226" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="227" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="228" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="229" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="230" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="231" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="232" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="233" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="234" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="235" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="236" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="237" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="238" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="239" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="240" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="241" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="242" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="243" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="244" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="245" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="246" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="247" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="248" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="249" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="250" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="251" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="252" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="253" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="254" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="255" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="256" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="257" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="258" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="259" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="260" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="261" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="262" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="263" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="264" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="265" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="266" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="267" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="268" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="269" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="270" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="271" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="272" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="273" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="274" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="275" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="276" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="277" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="278" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="279" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="280" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="281" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="282" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="283" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="284" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="285" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="286" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="287" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="288" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="289" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="290" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="291" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="292" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="293" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="294" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="295" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="296" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="297" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="298" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="299" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="300" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="301" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="302" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="303" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="304" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="305" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="306" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="307" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="308" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="309" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="310" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="311" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="312" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="313" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="314" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="315" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="316" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="317" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="318" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="319" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="320" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="321" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="322" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="323" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="324" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="325" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="326" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="327" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="328" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="329" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="330" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="331" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="332" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="333" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="334" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="335" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="336" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="337" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="338" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="339" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="340" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="341" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="342" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="343" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="344" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="345" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="346" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="347" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="348" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="349" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="350" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="351" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="352" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="353" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="354" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="355" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="356" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="357" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="358" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="359" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="360" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="361" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="362" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="363" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="364" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="365" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="366" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="367" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="368" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="369" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="370" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="371" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="372" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="373" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="374" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="375" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="376" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="377" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="378" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="379" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="380" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="381" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="382" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="383" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="384" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="385" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="386" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="387" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="388" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="389" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="390" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="391" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="392" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="393" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="394" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="395" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="396" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="397" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="398" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="399" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="400" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="401" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="402" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="403" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="404" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="405" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="406" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="407" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="408" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="409" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="410" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="411" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="412" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="413" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="414" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="415" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="416" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="417" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="418" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="419" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="420" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="421" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="422" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="423" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="424" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="425" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="426" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="427" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="428" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="429" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="430" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="431" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="432" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="433" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="434" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="435" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="436" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="437" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="438" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="439" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="440" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="441" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="442" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="443" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="444" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="445" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="446" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="447" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="448" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="449" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="450" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="451" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="452" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="453" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="454" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="455" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="456" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="457" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="458" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="459" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="460" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="461" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="462" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="463" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="464" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="465" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="466" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="467" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="468" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="469" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="470" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="471" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="472" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="473" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="474" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="475" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="476" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="477" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="478" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="479" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="480" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="481" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="482" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="483" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="484" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="485" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="486" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="487" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="488" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="489" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="490" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="491" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="492" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="493" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="494" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="495" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="496" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="497" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="498" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="499" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="500" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="501" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="502" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="503" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="504" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="505" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="506" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="507" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="508" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="509" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="510" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="511" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="512" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="513" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="514" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="515" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="516" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="517" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="518" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="519" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="520" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="521" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="522" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="523" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="524" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="525" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="526" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="527" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="528" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="529" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="530" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="531" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="532" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="533" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="534" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="535" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="536" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="537" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="538" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="539" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="540" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="541" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="542" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="543" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="544" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="545" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="546" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="547" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="548" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="549" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="550" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="551" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="552" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="553" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="554" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="555" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="556" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="557" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="558" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="559" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="560" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="561" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="562" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="563" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="564" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="565" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="566" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="567" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="568" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="569" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="570" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="571" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="572" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="573" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="574" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="575" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="576" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="577" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="578" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="579" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="580" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="581" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="582" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="583" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="584" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="585" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="586" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="587" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="588" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="589" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="590" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="591" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="592" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="593" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="594" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="595" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="596" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="597" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="598" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="599" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="600" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="601" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="602" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="603" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="604" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="605" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="606" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="607" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="608" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="609" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="610" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="611" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="612" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="613" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="614" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="615" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="616" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="617" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="618" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="619" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="620" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="621" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="622" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="623" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="624" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="625" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="626" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="627" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="628" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="629" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="630" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="631" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="632" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="633" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="634" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="635" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="636" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="637" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="638" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="639" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="640" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="641" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="642" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="643" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="644" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="645" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="646" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="647" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="648" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="649" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="650" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="651" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="652" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="653" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="654" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="655" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="656" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="657" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="658" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="659" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="660" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="661" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="662" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="663" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="664" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="665" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="666" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="667" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="668" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="669" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="670" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="671" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="672" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="673" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="674" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="675" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="676" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="677" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="678" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="679" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="680" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="681" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="682" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="683" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="684" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="685" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="686" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="687" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="688" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="689" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="690" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="691" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="692" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="693" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="694" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="695" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="696" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="697" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="698" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="699" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="700" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="701" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="702" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="703" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="704" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="705" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="706" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="707" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="708" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="709" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="710" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="711" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="712" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="713" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="714" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="715" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="716" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="717" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="718" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="719" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="720" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="721" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="722" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="723" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="724" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="725" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="726" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="727" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="728" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="729" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="730" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="731" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="732" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="733" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="734" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="735" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="736" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="737" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="738" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="739" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="740" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="741" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="742" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="743" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="744" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="745" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="746" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="747" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="748" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="749" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="750" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="751" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="752" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="753" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="754" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="755" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="756" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="757" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="758" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="759" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="760" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="761" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="762" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="763" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="764" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="765" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="766" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="767" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="768" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="769" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="770" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="771" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="772" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="773" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="774" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="775" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="776" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="777" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="778" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="779" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="780" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="781" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="782" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="783" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="784" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="785" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="786" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="787" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="788" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="789" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="790" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="791" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="792" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="793" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="794" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="795" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="796" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="797" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="798" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="799" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="800" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="801" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="802" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="803" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="804" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="805" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="806" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="807" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="808" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="809" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="810" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="811" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="812" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="813" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="814" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="815" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="816" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="817" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="818" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="819" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="820" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="821" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="822" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="823" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="824" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="825" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="826" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="827" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="828" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="829" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="830" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="831" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="832" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="833" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="834" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="835" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="836" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="837" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="838" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="839" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="840" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="841" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="842" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="843" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="844" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="845" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="846" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="847" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="848" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="849" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="850" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="851" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="852" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="853" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="854" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="855" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="856" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="857" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="858" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="859" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="860" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="861" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="862" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="863" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="864" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="865" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="866" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="867" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="868" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="869" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="870" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="871" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="872" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="873" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="874" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="875" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="876" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="877" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="878" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="879" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="880" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="881" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="882" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="883" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="884" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="885" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="886" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="887" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="888" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="889" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="890" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="891" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="892" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="893" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="894" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="895" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="896" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="897" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="898" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="899" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="900" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="901" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="902" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="903" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="904" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="905" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="906" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="907" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="908" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="909" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="910" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="911" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="912" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="913" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="914" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="915" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="916" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="917" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="918" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="919" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="920" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="921" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="922" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="923" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="924" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="925" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="926" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="927" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="928" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="929" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="930" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="931" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="932" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="933" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="934" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="935" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="936" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="937" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="938" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="939" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="940" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="941" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="942" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="943" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="944" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="945" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="946" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="947" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="948" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="949" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="950" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="951" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="952" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="953" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="954" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="955" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="956" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="957" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="958" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="959" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="960" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="961" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="962" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="963" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="964" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="965" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="966" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="967" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="968" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="969" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="970" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="971" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="972" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="973" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="974" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="975" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="976" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="977" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="978" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="979" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="980" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="981" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="982" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="983" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="984" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="985" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="986" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="987" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="988" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="989" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="990" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="991" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="992" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="993" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="994" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="995" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="996" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="997" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="998" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="999" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="1000" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="68" spans="2:23" ht="13.5" customHeight="1"/>
+    <row r="69" spans="2:23" ht="13.5" customHeight="1"/>
+    <row r="70" spans="2:23" ht="13.5" customHeight="1"/>
+    <row r="71" spans="2:23" ht="13.5" customHeight="1"/>
+    <row r="72" spans="2:23" ht="13.5" customHeight="1"/>
+    <row r="73" spans="2:23" ht="13.5" customHeight="1"/>
+    <row r="74" spans="2:23" ht="13.5" customHeight="1"/>
+    <row r="75" spans="2:23" ht="13.5" customHeight="1"/>
+    <row r="76" spans="2:23" ht="13.5" customHeight="1"/>
+    <row r="77" spans="2:23" ht="13.5" customHeight="1"/>
+    <row r="78" spans="2:23" ht="13.5" customHeight="1"/>
+    <row r="79" spans="2:23" ht="13.5" customHeight="1"/>
+    <row r="80" spans="2:23" ht="13.5" customHeight="1"/>
+    <row r="81" ht="13.5" customHeight="1"/>
+    <row r="82" ht="13.5" customHeight="1"/>
+    <row r="83" ht="13.5" customHeight="1"/>
+    <row r="84" ht="13.5" customHeight="1"/>
+    <row r="85" ht="13.5" customHeight="1"/>
+    <row r="86" ht="13.5" customHeight="1"/>
+    <row r="87" ht="13.5" customHeight="1"/>
+    <row r="88" ht="13.5" customHeight="1"/>
+    <row r="89" ht="13.5" customHeight="1"/>
+    <row r="90" ht="13.5" customHeight="1"/>
+    <row r="91" ht="13.5" customHeight="1"/>
+    <row r="92" ht="13.5" customHeight="1"/>
+    <row r="93" ht="13.5" customHeight="1"/>
+    <row r="94" ht="13.5" customHeight="1"/>
+    <row r="95" ht="13.5" customHeight="1"/>
+    <row r="96" ht="13.5" customHeight="1"/>
+    <row r="97" ht="13.5" customHeight="1"/>
+    <row r="98" ht="13.5" customHeight="1"/>
+    <row r="99" ht="13.5" customHeight="1"/>
+    <row r="100" ht="13.5" customHeight="1"/>
+    <row r="101" ht="13.5" customHeight="1"/>
+    <row r="102" ht="13.5" customHeight="1"/>
+    <row r="103" ht="13.5" customHeight="1"/>
+    <row r="104" ht="13.5" customHeight="1"/>
+    <row r="105" ht="13.5" customHeight="1"/>
+    <row r="106" ht="13.5" customHeight="1"/>
+    <row r="107" ht="13.5" customHeight="1"/>
+    <row r="108" ht="13.5" customHeight="1"/>
+    <row r="109" ht="13.5" customHeight="1"/>
+    <row r="110" ht="13.5" customHeight="1"/>
+    <row r="111" ht="13.5" customHeight="1"/>
+    <row r="112" ht="13.5" customHeight="1"/>
+    <row r="113" ht="13.5" customHeight="1"/>
+    <row r="114" ht="13.5" customHeight="1"/>
+    <row r="115" ht="13.5" customHeight="1"/>
+    <row r="116" ht="13.5" customHeight="1"/>
+    <row r="117" ht="13.5" customHeight="1"/>
+    <row r="118" ht="13.5" customHeight="1"/>
+    <row r="119" ht="13.5" customHeight="1"/>
+    <row r="120" ht="13.5" customHeight="1"/>
+    <row r="121" ht="13.5" customHeight="1"/>
+    <row r="122" ht="13.5" customHeight="1"/>
+    <row r="123" ht="13.5" customHeight="1"/>
+    <row r="124" ht="13.5" customHeight="1"/>
+    <row r="125" ht="13.5" customHeight="1"/>
+    <row r="126" ht="13.5" customHeight="1"/>
+    <row r="127" ht="13.5" customHeight="1"/>
+    <row r="128" ht="13.5" customHeight="1"/>
+    <row r="129" ht="13.5" customHeight="1"/>
+    <row r="130" ht="13.5" customHeight="1"/>
+    <row r="131" ht="13.5" customHeight="1"/>
+    <row r="132" ht="13.5" customHeight="1"/>
+    <row r="133" ht="13.5" customHeight="1"/>
+    <row r="134" ht="13.5" customHeight="1"/>
+    <row r="135" ht="13.5" customHeight="1"/>
+    <row r="136" ht="13.5" customHeight="1"/>
+    <row r="137" ht="13.5" customHeight="1"/>
+    <row r="138" ht="13.5" customHeight="1"/>
+    <row r="139" ht="13.5" customHeight="1"/>
+    <row r="140" ht="13.5" customHeight="1"/>
+    <row r="141" ht="13.5" customHeight="1"/>
+    <row r="142" ht="13.5" customHeight="1"/>
+    <row r="143" ht="13.5" customHeight="1"/>
+    <row r="144" ht="13.5" customHeight="1"/>
+    <row r="145" ht="13.5" customHeight="1"/>
+    <row r="146" ht="13.5" customHeight="1"/>
+    <row r="147" ht="13.5" customHeight="1"/>
+    <row r="148" ht="13.5" customHeight="1"/>
+    <row r="149" ht="13.5" customHeight="1"/>
+    <row r="150" ht="13.5" customHeight="1"/>
+    <row r="151" ht="13.5" customHeight="1"/>
+    <row r="152" ht="13.5" customHeight="1"/>
+    <row r="153" ht="13.5" customHeight="1"/>
+    <row r="154" ht="13.5" customHeight="1"/>
+    <row r="155" ht="13.5" customHeight="1"/>
+    <row r="156" ht="13.5" customHeight="1"/>
+    <row r="157" ht="13.5" customHeight="1"/>
+    <row r="158" ht="13.5" customHeight="1"/>
+    <row r="159" ht="13.5" customHeight="1"/>
+    <row r="160" ht="13.5" customHeight="1"/>
+    <row r="161" ht="13.5" customHeight="1"/>
+    <row r="162" ht="13.5" customHeight="1"/>
+    <row r="163" ht="13.5" customHeight="1"/>
+    <row r="164" ht="13.5" customHeight="1"/>
+    <row r="165" ht="13.5" customHeight="1"/>
+    <row r="166" ht="13.5" customHeight="1"/>
+    <row r="167" ht="13.5" customHeight="1"/>
+    <row r="168" ht="13.5" customHeight="1"/>
+    <row r="169" ht="13.5" customHeight="1"/>
+    <row r="170" ht="13.5" customHeight="1"/>
+    <row r="171" ht="13.5" customHeight="1"/>
+    <row r="172" ht="13.5" customHeight="1"/>
+    <row r="173" ht="13.5" customHeight="1"/>
+    <row r="174" ht="13.5" customHeight="1"/>
+    <row r="175" ht="13.5" customHeight="1"/>
+    <row r="176" ht="13.5" customHeight="1"/>
+    <row r="177" ht="13.5" customHeight="1"/>
+    <row r="178" ht="13.5" customHeight="1"/>
+    <row r="179" ht="13.5" customHeight="1"/>
+    <row r="180" ht="13.5" customHeight="1"/>
+    <row r="181" ht="13.5" customHeight="1"/>
+    <row r="182" ht="13.5" customHeight="1"/>
+    <row r="183" ht="13.5" customHeight="1"/>
+    <row r="184" ht="13.5" customHeight="1"/>
+    <row r="185" ht="13.5" customHeight="1"/>
+    <row r="186" ht="13.5" customHeight="1"/>
+    <row r="187" ht="13.5" customHeight="1"/>
+    <row r="188" ht="13.5" customHeight="1"/>
+    <row r="189" ht="13.5" customHeight="1"/>
+    <row r="190" ht="13.5" customHeight="1"/>
+    <row r="191" ht="13.5" customHeight="1"/>
+    <row r="192" ht="13.5" customHeight="1"/>
+    <row r="193" ht="13.5" customHeight="1"/>
+    <row r="194" ht="13.5" customHeight="1"/>
+    <row r="195" ht="13.5" customHeight="1"/>
+    <row r="196" ht="13.5" customHeight="1"/>
+    <row r="197" ht="13.5" customHeight="1"/>
+    <row r="198" ht="13.5" customHeight="1"/>
+    <row r="199" ht="13.5" customHeight="1"/>
+    <row r="200" ht="13.5" customHeight="1"/>
+    <row r="201" ht="13.5" customHeight="1"/>
+    <row r="202" ht="13.5" customHeight="1"/>
+    <row r="203" ht="13.5" customHeight="1"/>
+    <row r="204" ht="13.5" customHeight="1"/>
+    <row r="205" ht="13.5" customHeight="1"/>
+    <row r="206" ht="13.5" customHeight="1"/>
+    <row r="207" ht="13.5" customHeight="1"/>
+    <row r="208" ht="13.5" customHeight="1"/>
+    <row r="209" ht="13.5" customHeight="1"/>
+    <row r="210" ht="13.5" customHeight="1"/>
+    <row r="211" ht="13.5" customHeight="1"/>
+    <row r="212" ht="13.5" customHeight="1"/>
+    <row r="213" ht="13.5" customHeight="1"/>
+    <row r="214" ht="13.5" customHeight="1"/>
+    <row r="215" ht="13.5" customHeight="1"/>
+    <row r="216" ht="13.5" customHeight="1"/>
+    <row r="217" ht="13.5" customHeight="1"/>
+    <row r="218" ht="13.5" customHeight="1"/>
+    <row r="219" ht="13.5" customHeight="1"/>
+    <row r="220" ht="13.5" customHeight="1"/>
+    <row r="221" ht="13.5" customHeight="1"/>
+    <row r="222" ht="13.5" customHeight="1"/>
+    <row r="223" ht="13.5" customHeight="1"/>
+    <row r="224" ht="13.5" customHeight="1"/>
+    <row r="225" ht="13.5" customHeight="1"/>
+    <row r="226" ht="13.5" customHeight="1"/>
+    <row r="227" ht="13.5" customHeight="1"/>
+    <row r="228" ht="13.5" customHeight="1"/>
+    <row r="229" ht="13.5" customHeight="1"/>
+    <row r="230" ht="13.5" customHeight="1"/>
+    <row r="231" ht="13.5" customHeight="1"/>
+    <row r="232" ht="13.5" customHeight="1"/>
+    <row r="233" ht="13.5" customHeight="1"/>
+    <row r="234" ht="13.5" customHeight="1"/>
+    <row r="235" ht="13.5" customHeight="1"/>
+    <row r="236" ht="13.5" customHeight="1"/>
+    <row r="237" ht="13.5" customHeight="1"/>
+    <row r="238" ht="13.5" customHeight="1"/>
+    <row r="239" ht="13.5" customHeight="1"/>
+    <row r="240" ht="13.5" customHeight="1"/>
+    <row r="241" ht="13.5" customHeight="1"/>
+    <row r="242" ht="13.5" customHeight="1"/>
+    <row r="243" ht="13.5" customHeight="1"/>
+    <row r="244" ht="13.5" customHeight="1"/>
+    <row r="245" ht="13.5" customHeight="1"/>
+    <row r="246" ht="13.5" customHeight="1"/>
+    <row r="247" ht="13.5" customHeight="1"/>
+    <row r="248" ht="13.5" customHeight="1"/>
+    <row r="249" ht="13.5" customHeight="1"/>
+    <row r="250" ht="13.5" customHeight="1"/>
+    <row r="251" ht="13.5" customHeight="1"/>
+    <row r="252" ht="13.5" customHeight="1"/>
+    <row r="253" ht="13.5" customHeight="1"/>
+    <row r="254" ht="13.5" customHeight="1"/>
+    <row r="255" ht="13.5" customHeight="1"/>
+    <row r="256" ht="13.5" customHeight="1"/>
+    <row r="257" ht="13.5" customHeight="1"/>
+    <row r="258" ht="13.5" customHeight="1"/>
+    <row r="259" ht="13.5" customHeight="1"/>
+    <row r="260" ht="13.5" customHeight="1"/>
+    <row r="261" ht="13.5" customHeight="1"/>
+    <row r="262" ht="13.5" customHeight="1"/>
+    <row r="263" ht="13.5" customHeight="1"/>
+    <row r="264" ht="13.5" customHeight="1"/>
+    <row r="265" ht="13.5" customHeight="1"/>
+    <row r="266" ht="13.5" customHeight="1"/>
+    <row r="267" ht="13.5" customHeight="1"/>
+    <row r="268" ht="13.5" customHeight="1"/>
+    <row r="269" ht="13.5" customHeight="1"/>
+    <row r="270" ht="13.5" customHeight="1"/>
+    <row r="271" ht="13.5" customHeight="1"/>
+    <row r="272" ht="13.5" customHeight="1"/>
+    <row r="273" ht="13.5" customHeight="1"/>
+    <row r="274" ht="13.5" customHeight="1"/>
+    <row r="275" ht="13.5" customHeight="1"/>
+    <row r="276" ht="13.5" customHeight="1"/>
+    <row r="277" ht="13.5" customHeight="1"/>
+    <row r="278" ht="13.5" customHeight="1"/>
+    <row r="279" ht="13.5" customHeight="1"/>
+    <row r="280" ht="13.5" customHeight="1"/>
+    <row r="281" ht="13.5" customHeight="1"/>
+    <row r="282" ht="13.5" customHeight="1"/>
+    <row r="283" ht="13.5" customHeight="1"/>
+    <row r="284" ht="13.5" customHeight="1"/>
+    <row r="285" ht="13.5" customHeight="1"/>
+    <row r="286" ht="13.5" customHeight="1"/>
+    <row r="287" ht="13.5" customHeight="1"/>
+    <row r="288" ht="13.5" customHeight="1"/>
+    <row r="289" ht="13.5" customHeight="1"/>
+    <row r="290" ht="13.5" customHeight="1"/>
+    <row r="291" ht="13.5" customHeight="1"/>
+    <row r="292" ht="13.5" customHeight="1"/>
+    <row r="293" ht="13.5" customHeight="1"/>
+    <row r="294" ht="13.5" customHeight="1"/>
+    <row r="295" ht="13.5" customHeight="1"/>
+    <row r="296" ht="13.5" customHeight="1"/>
+    <row r="297" ht="13.5" customHeight="1"/>
+    <row r="298" ht="13.5" customHeight="1"/>
+    <row r="299" ht="13.5" customHeight="1"/>
+    <row r="300" ht="13.5" customHeight="1"/>
+    <row r="301" ht="13.5" customHeight="1"/>
+    <row r="302" ht="13.5" customHeight="1"/>
+    <row r="303" ht="13.5" customHeight="1"/>
+    <row r="304" ht="13.5" customHeight="1"/>
+    <row r="305" ht="13.5" customHeight="1"/>
+    <row r="306" ht="13.5" customHeight="1"/>
+    <row r="307" ht="13.5" customHeight="1"/>
+    <row r="308" ht="13.5" customHeight="1"/>
+    <row r="309" ht="13.5" customHeight="1"/>
+    <row r="310" ht="13.5" customHeight="1"/>
+    <row r="311" ht="13.5" customHeight="1"/>
+    <row r="312" ht="13.5" customHeight="1"/>
+    <row r="313" ht="13.5" customHeight="1"/>
+    <row r="314" ht="13.5" customHeight="1"/>
+    <row r="315" ht="13.5" customHeight="1"/>
+    <row r="316" ht="13.5" customHeight="1"/>
+    <row r="317" ht="13.5" customHeight="1"/>
+    <row r="318" ht="13.5" customHeight="1"/>
+    <row r="319" ht="13.5" customHeight="1"/>
+    <row r="320" ht="13.5" customHeight="1"/>
+    <row r="321" ht="13.5" customHeight="1"/>
+    <row r="322" ht="13.5" customHeight="1"/>
+    <row r="323" ht="13.5" customHeight="1"/>
+    <row r="324" ht="13.5" customHeight="1"/>
+    <row r="325" ht="13.5" customHeight="1"/>
+    <row r="326" ht="13.5" customHeight="1"/>
+    <row r="327" ht="13.5" customHeight="1"/>
+    <row r="328" ht="13.5" customHeight="1"/>
+    <row r="329" ht="13.5" customHeight="1"/>
+    <row r="330" ht="13.5" customHeight="1"/>
+    <row r="331" ht="13.5" customHeight="1"/>
+    <row r="332" ht="13.5" customHeight="1"/>
+    <row r="333" ht="13.5" customHeight="1"/>
+    <row r="334" ht="13.5" customHeight="1"/>
+    <row r="335" ht="13.5" customHeight="1"/>
+    <row r="336" ht="13.5" customHeight="1"/>
+    <row r="337" ht="13.5" customHeight="1"/>
+    <row r="338" ht="13.5" customHeight="1"/>
+    <row r="339" ht="13.5" customHeight="1"/>
+    <row r="340" ht="13.5" customHeight="1"/>
+    <row r="341" ht="13.5" customHeight="1"/>
+    <row r="342" ht="13.5" customHeight="1"/>
+    <row r="343" ht="13.5" customHeight="1"/>
+    <row r="344" ht="13.5" customHeight="1"/>
+    <row r="345" ht="13.5" customHeight="1"/>
+    <row r="346" ht="13.5" customHeight="1"/>
+    <row r="347" ht="13.5" customHeight="1"/>
+    <row r="348" ht="13.5" customHeight="1"/>
+    <row r="349" ht="13.5" customHeight="1"/>
+    <row r="350" ht="13.5" customHeight="1"/>
+    <row r="351" ht="13.5" customHeight="1"/>
+    <row r="352" ht="13.5" customHeight="1"/>
+    <row r="353" ht="13.5" customHeight="1"/>
+    <row r="354" ht="13.5" customHeight="1"/>
+    <row r="355" ht="13.5" customHeight="1"/>
+    <row r="356" ht="13.5" customHeight="1"/>
+    <row r="357" ht="13.5" customHeight="1"/>
+    <row r="358" ht="13.5" customHeight="1"/>
+    <row r="359" ht="13.5" customHeight="1"/>
+    <row r="360" ht="13.5" customHeight="1"/>
+    <row r="361" ht="13.5" customHeight="1"/>
+    <row r="362" ht="13.5" customHeight="1"/>
+    <row r="363" ht="13.5" customHeight="1"/>
+    <row r="364" ht="13.5" customHeight="1"/>
+    <row r="365" ht="13.5" customHeight="1"/>
+    <row r="366" ht="13.5" customHeight="1"/>
+    <row r="367" ht="13.5" customHeight="1"/>
+    <row r="368" ht="13.5" customHeight="1"/>
+    <row r="369" ht="13.5" customHeight="1"/>
+    <row r="370" ht="13.5" customHeight="1"/>
+    <row r="371" ht="13.5" customHeight="1"/>
+    <row r="372" ht="13.5" customHeight="1"/>
+    <row r="373" ht="13.5" customHeight="1"/>
+    <row r="374" ht="13.5" customHeight="1"/>
+    <row r="375" ht="13.5" customHeight="1"/>
+    <row r="376" ht="13.5" customHeight="1"/>
+    <row r="377" ht="13.5" customHeight="1"/>
+    <row r="378" ht="13.5" customHeight="1"/>
+    <row r="379" ht="13.5" customHeight="1"/>
+    <row r="380" ht="13.5" customHeight="1"/>
+    <row r="381" ht="13.5" customHeight="1"/>
+    <row r="382" ht="13.5" customHeight="1"/>
+    <row r="383" ht="13.5" customHeight="1"/>
+    <row r="384" ht="13.5" customHeight="1"/>
+    <row r="385" ht="13.5" customHeight="1"/>
+    <row r="386" ht="13.5" customHeight="1"/>
+    <row r="387" ht="13.5" customHeight="1"/>
+    <row r="388" ht="13.5" customHeight="1"/>
+    <row r="389" ht="13.5" customHeight="1"/>
+    <row r="390" ht="13.5" customHeight="1"/>
+    <row r="391" ht="13.5" customHeight="1"/>
+    <row r="392" ht="13.5" customHeight="1"/>
+    <row r="393" ht="13.5" customHeight="1"/>
+    <row r="394" ht="13.5" customHeight="1"/>
+    <row r="395" ht="13.5" customHeight="1"/>
+    <row r="396" ht="13.5" customHeight="1"/>
+    <row r="397" ht="13.5" customHeight="1"/>
+    <row r="398" ht="13.5" customHeight="1"/>
+    <row r="399" ht="13.5" customHeight="1"/>
+    <row r="400" ht="13.5" customHeight="1"/>
+    <row r="401" ht="13.5" customHeight="1"/>
+    <row r="402" ht="13.5" customHeight="1"/>
+    <row r="403" ht="13.5" customHeight="1"/>
+    <row r="404" ht="13.5" customHeight="1"/>
+    <row r="405" ht="13.5" customHeight="1"/>
+    <row r="406" ht="13.5" customHeight="1"/>
+    <row r="407" ht="13.5" customHeight="1"/>
+    <row r="408" ht="13.5" customHeight="1"/>
+    <row r="409" ht="13.5" customHeight="1"/>
+    <row r="410" ht="13.5" customHeight="1"/>
+    <row r="411" ht="13.5" customHeight="1"/>
+    <row r="412" ht="13.5" customHeight="1"/>
+    <row r="413" ht="13.5" customHeight="1"/>
+    <row r="414" ht="13.5" customHeight="1"/>
+    <row r="415" ht="13.5" customHeight="1"/>
+    <row r="416" ht="13.5" customHeight="1"/>
+    <row r="417" ht="13.5" customHeight="1"/>
+    <row r="418" ht="13.5" customHeight="1"/>
+    <row r="419" ht="13.5" customHeight="1"/>
+    <row r="420" ht="13.5" customHeight="1"/>
+    <row r="421" ht="13.5" customHeight="1"/>
+    <row r="422" ht="13.5" customHeight="1"/>
+    <row r="423" ht="13.5" customHeight="1"/>
+    <row r="424" ht="13.5" customHeight="1"/>
+    <row r="425" ht="13.5" customHeight="1"/>
+    <row r="426" ht="13.5" customHeight="1"/>
+    <row r="427" ht="13.5" customHeight="1"/>
+    <row r="428" ht="13.5" customHeight="1"/>
+    <row r="429" ht="13.5" customHeight="1"/>
+    <row r="430" ht="13.5" customHeight="1"/>
+    <row r="431" ht="13.5" customHeight="1"/>
+    <row r="432" ht="13.5" customHeight="1"/>
+    <row r="433" ht="13.5" customHeight="1"/>
+    <row r="434" ht="13.5" customHeight="1"/>
+    <row r="435" ht="13.5" customHeight="1"/>
+    <row r="436" ht="13.5" customHeight="1"/>
+    <row r="437" ht="13.5" customHeight="1"/>
+    <row r="438" ht="13.5" customHeight="1"/>
+    <row r="439" ht="13.5" customHeight="1"/>
+    <row r="440" ht="13.5" customHeight="1"/>
+    <row r="441" ht="13.5" customHeight="1"/>
+    <row r="442" ht="13.5" customHeight="1"/>
+    <row r="443" ht="13.5" customHeight="1"/>
+    <row r="444" ht="13.5" customHeight="1"/>
+    <row r="445" ht="13.5" customHeight="1"/>
+    <row r="446" ht="13.5" customHeight="1"/>
+    <row r="447" ht="13.5" customHeight="1"/>
+    <row r="448" ht="13.5" customHeight="1"/>
+    <row r="449" ht="13.5" customHeight="1"/>
+    <row r="450" ht="13.5" customHeight="1"/>
+    <row r="451" ht="13.5" customHeight="1"/>
+    <row r="452" ht="13.5" customHeight="1"/>
+    <row r="453" ht="13.5" customHeight="1"/>
+    <row r="454" ht="13.5" customHeight="1"/>
+    <row r="455" ht="13.5" customHeight="1"/>
+    <row r="456" ht="13.5" customHeight="1"/>
+    <row r="457" ht="13.5" customHeight="1"/>
+    <row r="458" ht="13.5" customHeight="1"/>
+    <row r="459" ht="13.5" customHeight="1"/>
+    <row r="460" ht="13.5" customHeight="1"/>
+    <row r="461" ht="13.5" customHeight="1"/>
+    <row r="462" ht="13.5" customHeight="1"/>
+    <row r="463" ht="13.5" customHeight="1"/>
+    <row r="464" ht="13.5" customHeight="1"/>
+    <row r="465" ht="13.5" customHeight="1"/>
+    <row r="466" ht="13.5" customHeight="1"/>
+    <row r="467" ht="13.5" customHeight="1"/>
+    <row r="468" ht="13.5" customHeight="1"/>
+    <row r="469" ht="13.5" customHeight="1"/>
+    <row r="470" ht="13.5" customHeight="1"/>
+    <row r="471" ht="13.5" customHeight="1"/>
+    <row r="472" ht="13.5" customHeight="1"/>
+    <row r="473" ht="13.5" customHeight="1"/>
+    <row r="474" ht="13.5" customHeight="1"/>
+    <row r="475" ht="13.5" customHeight="1"/>
+    <row r="476" ht="13.5" customHeight="1"/>
+    <row r="477" ht="13.5" customHeight="1"/>
+    <row r="478" ht="13.5" customHeight="1"/>
+    <row r="479" ht="13.5" customHeight="1"/>
+    <row r="480" ht="13.5" customHeight="1"/>
+    <row r="481" ht="13.5" customHeight="1"/>
+    <row r="482" ht="13.5" customHeight="1"/>
+    <row r="483" ht="13.5" customHeight="1"/>
+    <row r="484" ht="13.5" customHeight="1"/>
+    <row r="485" ht="13.5" customHeight="1"/>
+    <row r="486" ht="13.5" customHeight="1"/>
+    <row r="487" ht="13.5" customHeight="1"/>
+    <row r="488" ht="13.5" customHeight="1"/>
+    <row r="489" ht="13.5" customHeight="1"/>
+    <row r="490" ht="13.5" customHeight="1"/>
+    <row r="491" ht="13.5" customHeight="1"/>
+    <row r="492" ht="13.5" customHeight="1"/>
+    <row r="493" ht="13.5" customHeight="1"/>
+    <row r="494" ht="13.5" customHeight="1"/>
+    <row r="495" ht="13.5" customHeight="1"/>
+    <row r="496" ht="13.5" customHeight="1"/>
+    <row r="497" ht="13.5" customHeight="1"/>
+    <row r="498" ht="13.5" customHeight="1"/>
+    <row r="499" ht="13.5" customHeight="1"/>
+    <row r="500" ht="13.5" customHeight="1"/>
+    <row r="501" ht="13.5" customHeight="1"/>
+    <row r="502" ht="13.5" customHeight="1"/>
+    <row r="503" ht="13.5" customHeight="1"/>
+    <row r="504" ht="13.5" customHeight="1"/>
+    <row r="505" ht="13.5" customHeight="1"/>
+    <row r="506" ht="13.5" customHeight="1"/>
+    <row r="507" ht="13.5" customHeight="1"/>
+    <row r="508" ht="13.5" customHeight="1"/>
+    <row r="509" ht="13.5" customHeight="1"/>
+    <row r="510" ht="13.5" customHeight="1"/>
+    <row r="511" ht="13.5" customHeight="1"/>
+    <row r="512" ht="13.5" customHeight="1"/>
+    <row r="513" ht="13.5" customHeight="1"/>
+    <row r="514" ht="13.5" customHeight="1"/>
+    <row r="515" ht="13.5" customHeight="1"/>
+    <row r="516" ht="13.5" customHeight="1"/>
+    <row r="517" ht="13.5" customHeight="1"/>
+    <row r="518" ht="13.5" customHeight="1"/>
+    <row r="519" ht="13.5" customHeight="1"/>
+    <row r="520" ht="13.5" customHeight="1"/>
+    <row r="521" ht="13.5" customHeight="1"/>
+    <row r="522" ht="13.5" customHeight="1"/>
+    <row r="523" ht="13.5" customHeight="1"/>
+    <row r="524" ht="13.5" customHeight="1"/>
+    <row r="525" ht="13.5" customHeight="1"/>
+    <row r="526" ht="13.5" customHeight="1"/>
+    <row r="527" ht="13.5" customHeight="1"/>
+    <row r="528" ht="13.5" customHeight="1"/>
+    <row r="529" ht="13.5" customHeight="1"/>
+    <row r="530" ht="13.5" customHeight="1"/>
+    <row r="531" ht="13.5" customHeight="1"/>
+    <row r="532" ht="13.5" customHeight="1"/>
+    <row r="533" ht="13.5" customHeight="1"/>
+    <row r="534" ht="13.5" customHeight="1"/>
+    <row r="535" ht="13.5" customHeight="1"/>
+    <row r="536" ht="13.5" customHeight="1"/>
+    <row r="537" ht="13.5" customHeight="1"/>
+    <row r="538" ht="13.5" customHeight="1"/>
+    <row r="539" ht="13.5" customHeight="1"/>
+    <row r="540" ht="13.5" customHeight="1"/>
+    <row r="541" ht="13.5" customHeight="1"/>
+    <row r="542" ht="13.5" customHeight="1"/>
+    <row r="543" ht="13.5" customHeight="1"/>
+    <row r="544" ht="13.5" customHeight="1"/>
+    <row r="545" ht="13.5" customHeight="1"/>
+    <row r="546" ht="13.5" customHeight="1"/>
+    <row r="547" ht="13.5" customHeight="1"/>
+    <row r="548" ht="13.5" customHeight="1"/>
+    <row r="549" ht="13.5" customHeight="1"/>
+    <row r="550" ht="13.5" customHeight="1"/>
+    <row r="551" ht="13.5" customHeight="1"/>
+    <row r="552" ht="13.5" customHeight="1"/>
+    <row r="553" ht="13.5" customHeight="1"/>
+    <row r="554" ht="13.5" customHeight="1"/>
+    <row r="555" ht="13.5" customHeight="1"/>
+    <row r="556" ht="13.5" customHeight="1"/>
+    <row r="557" ht="13.5" customHeight="1"/>
+    <row r="558" ht="13.5" customHeight="1"/>
+    <row r="559" ht="13.5" customHeight="1"/>
+    <row r="560" ht="13.5" customHeight="1"/>
+    <row r="561" ht="13.5" customHeight="1"/>
+    <row r="562" ht="13.5" customHeight="1"/>
+    <row r="563" ht="13.5" customHeight="1"/>
+    <row r="564" ht="13.5" customHeight="1"/>
+    <row r="565" ht="13.5" customHeight="1"/>
+    <row r="566" ht="13.5" customHeight="1"/>
+    <row r="567" ht="13.5" customHeight="1"/>
+    <row r="568" ht="13.5" customHeight="1"/>
+    <row r="569" ht="13.5" customHeight="1"/>
+    <row r="570" ht="13.5" customHeight="1"/>
+    <row r="571" ht="13.5" customHeight="1"/>
+    <row r="572" ht="13.5" customHeight="1"/>
+    <row r="573" ht="13.5" customHeight="1"/>
+    <row r="574" ht="13.5" customHeight="1"/>
+    <row r="575" ht="13.5" customHeight="1"/>
+    <row r="576" ht="13.5" customHeight="1"/>
+    <row r="577" ht="13.5" customHeight="1"/>
+    <row r="578" ht="13.5" customHeight="1"/>
+    <row r="579" ht="13.5" customHeight="1"/>
+    <row r="580" ht="13.5" customHeight="1"/>
+    <row r="581" ht="13.5" customHeight="1"/>
+    <row r="582" ht="13.5" customHeight="1"/>
+    <row r="583" ht="13.5" customHeight="1"/>
+    <row r="584" ht="13.5" customHeight="1"/>
+    <row r="585" ht="13.5" customHeight="1"/>
+    <row r="586" ht="13.5" customHeight="1"/>
+    <row r="587" ht="13.5" customHeight="1"/>
+    <row r="588" ht="13.5" customHeight="1"/>
+    <row r="589" ht="13.5" customHeight="1"/>
+    <row r="590" ht="13.5" customHeight="1"/>
+    <row r="591" ht="13.5" customHeight="1"/>
+    <row r="592" ht="13.5" customHeight="1"/>
+    <row r="593" ht="13.5" customHeight="1"/>
+    <row r="594" ht="13.5" customHeight="1"/>
+    <row r="595" ht="13.5" customHeight="1"/>
+    <row r="596" ht="13.5" customHeight="1"/>
+    <row r="597" ht="13.5" customHeight="1"/>
+    <row r="598" ht="13.5" customHeight="1"/>
+    <row r="599" ht="13.5" customHeight="1"/>
+    <row r="600" ht="13.5" customHeight="1"/>
+    <row r="601" ht="13.5" customHeight="1"/>
+    <row r="602" ht="13.5" customHeight="1"/>
+    <row r="603" ht="13.5" customHeight="1"/>
+    <row r="604" ht="13.5" customHeight="1"/>
+    <row r="605" ht="13.5" customHeight="1"/>
+    <row r="606" ht="13.5" customHeight="1"/>
+    <row r="607" ht="13.5" customHeight="1"/>
+    <row r="608" ht="13.5" customHeight="1"/>
+    <row r="609" ht="13.5" customHeight="1"/>
+    <row r="610" ht="13.5" customHeight="1"/>
+    <row r="611" ht="13.5" customHeight="1"/>
+    <row r="612" ht="13.5" customHeight="1"/>
+    <row r="613" ht="13.5" customHeight="1"/>
+    <row r="614" ht="13.5" customHeight="1"/>
+    <row r="615" ht="13.5" customHeight="1"/>
+    <row r="616" ht="13.5" customHeight="1"/>
+    <row r="617" ht="13.5" customHeight="1"/>
+    <row r="618" ht="13.5" customHeight="1"/>
+    <row r="619" ht="13.5" customHeight="1"/>
+    <row r="620" ht="13.5" customHeight="1"/>
+    <row r="621" ht="13.5" customHeight="1"/>
+    <row r="622" ht="13.5" customHeight="1"/>
+    <row r="623" ht="13.5" customHeight="1"/>
+    <row r="624" ht="13.5" customHeight="1"/>
+    <row r="625" ht="13.5" customHeight="1"/>
+    <row r="626" ht="13.5" customHeight="1"/>
+    <row r="627" ht="13.5" customHeight="1"/>
+    <row r="628" ht="13.5" customHeight="1"/>
+    <row r="629" ht="13.5" customHeight="1"/>
+    <row r="630" ht="13.5" customHeight="1"/>
+    <row r="631" ht="13.5" customHeight="1"/>
+    <row r="632" ht="13.5" customHeight="1"/>
+    <row r="633" ht="13.5" customHeight="1"/>
+    <row r="634" ht="13.5" customHeight="1"/>
+    <row r="635" ht="13.5" customHeight="1"/>
+    <row r="636" ht="13.5" customHeight="1"/>
+    <row r="637" ht="13.5" customHeight="1"/>
+    <row r="638" ht="13.5" customHeight="1"/>
+    <row r="639" ht="13.5" customHeight="1"/>
+    <row r="640" ht="13.5" customHeight="1"/>
+    <row r="641" ht="13.5" customHeight="1"/>
+    <row r="642" ht="13.5" customHeight="1"/>
+    <row r="643" ht="13.5" customHeight="1"/>
+    <row r="644" ht="13.5" customHeight="1"/>
+    <row r="645" ht="13.5" customHeight="1"/>
+    <row r="646" ht="13.5" customHeight="1"/>
+    <row r="647" ht="13.5" customHeight="1"/>
+    <row r="648" ht="13.5" customHeight="1"/>
+    <row r="649" ht="13.5" customHeight="1"/>
+    <row r="650" ht="13.5" customHeight="1"/>
+    <row r="651" ht="13.5" customHeight="1"/>
+    <row r="652" ht="13.5" customHeight="1"/>
+    <row r="653" ht="13.5" customHeight="1"/>
+    <row r="654" ht="13.5" customHeight="1"/>
+    <row r="655" ht="13.5" customHeight="1"/>
+    <row r="656" ht="13.5" customHeight="1"/>
+    <row r="657" ht="13.5" customHeight="1"/>
+    <row r="658" ht="13.5" customHeight="1"/>
+    <row r="659" ht="13.5" customHeight="1"/>
+    <row r="660" ht="13.5" customHeight="1"/>
+    <row r="661" ht="13.5" customHeight="1"/>
+    <row r="662" ht="13.5" customHeight="1"/>
+    <row r="663" ht="13.5" customHeight="1"/>
+    <row r="664" ht="13.5" customHeight="1"/>
+    <row r="665" ht="13.5" customHeight="1"/>
+    <row r="666" ht="13.5" customHeight="1"/>
+    <row r="667" ht="13.5" customHeight="1"/>
+    <row r="668" ht="13.5" customHeight="1"/>
+    <row r="669" ht="13.5" customHeight="1"/>
+    <row r="670" ht="13.5" customHeight="1"/>
+    <row r="671" ht="13.5" customHeight="1"/>
+    <row r="672" ht="13.5" customHeight="1"/>
+    <row r="673" ht="13.5" customHeight="1"/>
+    <row r="674" ht="13.5" customHeight="1"/>
+    <row r="675" ht="13.5" customHeight="1"/>
+    <row r="676" ht="13.5" customHeight="1"/>
+    <row r="677" ht="13.5" customHeight="1"/>
+    <row r="678" ht="13.5" customHeight="1"/>
+    <row r="679" ht="13.5" customHeight="1"/>
+    <row r="680" ht="13.5" customHeight="1"/>
+    <row r="681" ht="13.5" customHeight="1"/>
+    <row r="682" ht="13.5" customHeight="1"/>
+    <row r="683" ht="13.5" customHeight="1"/>
+    <row r="684" ht="13.5" customHeight="1"/>
+    <row r="685" ht="13.5" customHeight="1"/>
+    <row r="686" ht="13.5" customHeight="1"/>
+    <row r="687" ht="13.5" customHeight="1"/>
+    <row r="688" ht="13.5" customHeight="1"/>
+    <row r="689" ht="13.5" customHeight="1"/>
+    <row r="690" ht="13.5" customHeight="1"/>
+    <row r="691" ht="13.5" customHeight="1"/>
+    <row r="692" ht="13.5" customHeight="1"/>
+    <row r="693" ht="13.5" customHeight="1"/>
+    <row r="694" ht="13.5" customHeight="1"/>
+    <row r="695" ht="13.5" customHeight="1"/>
+    <row r="696" ht="13.5" customHeight="1"/>
+    <row r="697" ht="13.5" customHeight="1"/>
+    <row r="698" ht="13.5" customHeight="1"/>
+    <row r="699" ht="13.5" customHeight="1"/>
+    <row r="700" ht="13.5" customHeight="1"/>
+    <row r="701" ht="13.5" customHeight="1"/>
+    <row r="702" ht="13.5" customHeight="1"/>
+    <row r="703" ht="13.5" customHeight="1"/>
+    <row r="704" ht="13.5" customHeight="1"/>
+    <row r="705" ht="13.5" customHeight="1"/>
+    <row r="706" ht="13.5" customHeight="1"/>
+    <row r="707" ht="13.5" customHeight="1"/>
+    <row r="708" ht="13.5" customHeight="1"/>
+    <row r="709" ht="13.5" customHeight="1"/>
+    <row r="710" ht="13.5" customHeight="1"/>
+    <row r="711" ht="13.5" customHeight="1"/>
+    <row r="712" ht="13.5" customHeight="1"/>
+    <row r="713" ht="13.5" customHeight="1"/>
+    <row r="714" ht="13.5" customHeight="1"/>
+    <row r="715" ht="13.5" customHeight="1"/>
+    <row r="716" ht="13.5" customHeight="1"/>
+    <row r="717" ht="13.5" customHeight="1"/>
+    <row r="718" ht="13.5" customHeight="1"/>
+    <row r="719" ht="13.5" customHeight="1"/>
+    <row r="720" ht="13.5" customHeight="1"/>
+    <row r="721" ht="13.5" customHeight="1"/>
+    <row r="722" ht="13.5" customHeight="1"/>
+    <row r="723" ht="13.5" customHeight="1"/>
+    <row r="724" ht="13.5" customHeight="1"/>
+    <row r="725" ht="13.5" customHeight="1"/>
+    <row r="726" ht="13.5" customHeight="1"/>
+    <row r="727" ht="13.5" customHeight="1"/>
+    <row r="728" ht="13.5" customHeight="1"/>
+    <row r="729" ht="13.5" customHeight="1"/>
+    <row r="730" ht="13.5" customHeight="1"/>
+    <row r="731" ht="13.5" customHeight="1"/>
+    <row r="732" ht="13.5" customHeight="1"/>
+    <row r="733" ht="13.5" customHeight="1"/>
+    <row r="734" ht="13.5" customHeight="1"/>
+    <row r="735" ht="13.5" customHeight="1"/>
+    <row r="736" ht="13.5" customHeight="1"/>
+    <row r="737" ht="13.5" customHeight="1"/>
+    <row r="738" ht="13.5" customHeight="1"/>
+    <row r="739" ht="13.5" customHeight="1"/>
+    <row r="740" ht="13.5" customHeight="1"/>
+    <row r="741" ht="13.5" customHeight="1"/>
+    <row r="742" ht="13.5" customHeight="1"/>
+    <row r="743" ht="13.5" customHeight="1"/>
+    <row r="744" ht="13.5" customHeight="1"/>
+    <row r="745" ht="13.5" customHeight="1"/>
+    <row r="746" ht="13.5" customHeight="1"/>
+    <row r="747" ht="13.5" customHeight="1"/>
+    <row r="748" ht="13.5" customHeight="1"/>
+    <row r="749" ht="13.5" customHeight="1"/>
+    <row r="750" ht="13.5" customHeight="1"/>
+    <row r="751" ht="13.5" customHeight="1"/>
+    <row r="752" ht="13.5" customHeight="1"/>
+    <row r="753" ht="13.5" customHeight="1"/>
+    <row r="754" ht="13.5" customHeight="1"/>
+    <row r="755" ht="13.5" customHeight="1"/>
+    <row r="756" ht="13.5" customHeight="1"/>
+    <row r="757" ht="13.5" customHeight="1"/>
+    <row r="758" ht="13.5" customHeight="1"/>
+    <row r="759" ht="13.5" customHeight="1"/>
+    <row r="760" ht="13.5" customHeight="1"/>
+    <row r="761" ht="13.5" customHeight="1"/>
+    <row r="762" ht="13.5" customHeight="1"/>
+    <row r="763" ht="13.5" customHeight="1"/>
+    <row r="764" ht="13.5" customHeight="1"/>
+    <row r="765" ht="13.5" customHeight="1"/>
+    <row r="766" ht="13.5" customHeight="1"/>
+    <row r="767" ht="13.5" customHeight="1"/>
+    <row r="768" ht="13.5" customHeight="1"/>
+    <row r="769" ht="13.5" customHeight="1"/>
+    <row r="770" ht="13.5" customHeight="1"/>
+    <row r="771" ht="13.5" customHeight="1"/>
+    <row r="772" ht="13.5" customHeight="1"/>
+    <row r="773" ht="13.5" customHeight="1"/>
+    <row r="774" ht="13.5" customHeight="1"/>
+    <row r="775" ht="13.5" customHeight="1"/>
+    <row r="776" ht="13.5" customHeight="1"/>
+    <row r="777" ht="13.5" customHeight="1"/>
+    <row r="778" ht="13.5" customHeight="1"/>
+    <row r="779" ht="13.5" customHeight="1"/>
+    <row r="780" ht="13.5" customHeight="1"/>
+    <row r="781" ht="13.5" customHeight="1"/>
+    <row r="782" ht="13.5" customHeight="1"/>
+    <row r="783" ht="13.5" customHeight="1"/>
+    <row r="784" ht="13.5" customHeight="1"/>
+    <row r="785" ht="13.5" customHeight="1"/>
+    <row r="786" ht="13.5" customHeight="1"/>
+    <row r="787" ht="13.5" customHeight="1"/>
+    <row r="788" ht="13.5" customHeight="1"/>
+    <row r="789" ht="13.5" customHeight="1"/>
+    <row r="790" ht="13.5" customHeight="1"/>
+    <row r="791" ht="13.5" customHeight="1"/>
+    <row r="792" ht="13.5" customHeight="1"/>
+    <row r="793" ht="13.5" customHeight="1"/>
+    <row r="794" ht="13.5" customHeight="1"/>
+    <row r="795" ht="13.5" customHeight="1"/>
+    <row r="796" ht="13.5" customHeight="1"/>
+    <row r="797" ht="13.5" customHeight="1"/>
+    <row r="798" ht="13.5" customHeight="1"/>
+    <row r="799" ht="13.5" customHeight="1"/>
+    <row r="800" ht="13.5" customHeight="1"/>
+    <row r="801" ht="13.5" customHeight="1"/>
+    <row r="802" ht="13.5" customHeight="1"/>
+    <row r="803" ht="13.5" customHeight="1"/>
+    <row r="804" ht="13.5" customHeight="1"/>
+    <row r="805" ht="13.5" customHeight="1"/>
+    <row r="806" ht="13.5" customHeight="1"/>
+    <row r="807" ht="13.5" customHeight="1"/>
+    <row r="808" ht="13.5" customHeight="1"/>
+    <row r="809" ht="13.5" customHeight="1"/>
+    <row r="810" ht="13.5" customHeight="1"/>
+    <row r="811" ht="13.5" customHeight="1"/>
+    <row r="812" ht="13.5" customHeight="1"/>
+    <row r="813" ht="13.5" customHeight="1"/>
+    <row r="814" ht="13.5" customHeight="1"/>
+    <row r="815" ht="13.5" customHeight="1"/>
+    <row r="816" ht="13.5" customHeight="1"/>
+    <row r="817" ht="13.5" customHeight="1"/>
+    <row r="818" ht="13.5" customHeight="1"/>
+    <row r="819" ht="13.5" customHeight="1"/>
+    <row r="820" ht="13.5" customHeight="1"/>
+    <row r="821" ht="13.5" customHeight="1"/>
+    <row r="822" ht="13.5" customHeight="1"/>
+    <row r="823" ht="13.5" customHeight="1"/>
+    <row r="824" ht="13.5" customHeight="1"/>
+    <row r="825" ht="13.5" customHeight="1"/>
+    <row r="826" ht="13.5" customHeight="1"/>
+    <row r="827" ht="13.5" customHeight="1"/>
+    <row r="828" ht="13.5" customHeight="1"/>
+    <row r="829" ht="13.5" customHeight="1"/>
+    <row r="830" ht="13.5" customHeight="1"/>
+    <row r="831" ht="13.5" customHeight="1"/>
+    <row r="832" ht="13.5" customHeight="1"/>
+    <row r="833" ht="13.5" customHeight="1"/>
+    <row r="834" ht="13.5" customHeight="1"/>
+    <row r="835" ht="13.5" customHeight="1"/>
+    <row r="836" ht="13.5" customHeight="1"/>
+    <row r="837" ht="13.5" customHeight="1"/>
+    <row r="838" ht="13.5" customHeight="1"/>
+    <row r="839" ht="13.5" customHeight="1"/>
+    <row r="840" ht="13.5" customHeight="1"/>
+    <row r="841" ht="13.5" customHeight="1"/>
+    <row r="842" ht="13.5" customHeight="1"/>
+    <row r="843" ht="13.5" customHeight="1"/>
+    <row r="844" ht="13.5" customHeight="1"/>
+    <row r="845" ht="13.5" customHeight="1"/>
+    <row r="846" ht="13.5" customHeight="1"/>
+    <row r="847" ht="13.5" customHeight="1"/>
+    <row r="848" ht="13.5" customHeight="1"/>
+    <row r="849" ht="13.5" customHeight="1"/>
+    <row r="850" ht="13.5" customHeight="1"/>
+    <row r="851" ht="13.5" customHeight="1"/>
+    <row r="852" ht="13.5" customHeight="1"/>
+    <row r="853" ht="13.5" customHeight="1"/>
+    <row r="854" ht="13.5" customHeight="1"/>
+    <row r="855" ht="13.5" customHeight="1"/>
+    <row r="856" ht="13.5" customHeight="1"/>
+    <row r="857" ht="13.5" customHeight="1"/>
+    <row r="858" ht="13.5" customHeight="1"/>
+    <row r="859" ht="13.5" customHeight="1"/>
+    <row r="860" ht="13.5" customHeight="1"/>
+    <row r="861" ht="13.5" customHeight="1"/>
+    <row r="862" ht="13.5" customHeight="1"/>
+    <row r="863" ht="13.5" customHeight="1"/>
+    <row r="864" ht="13.5" customHeight="1"/>
+    <row r="865" ht="13.5" customHeight="1"/>
+    <row r="866" ht="13.5" customHeight="1"/>
+    <row r="867" ht="13.5" customHeight="1"/>
+    <row r="868" ht="13.5" customHeight="1"/>
+    <row r="869" ht="13.5" customHeight="1"/>
+    <row r="870" ht="13.5" customHeight="1"/>
+    <row r="871" ht="13.5" customHeight="1"/>
+    <row r="872" ht="13.5" customHeight="1"/>
+    <row r="873" ht="13.5" customHeight="1"/>
+    <row r="874" ht="13.5" customHeight="1"/>
+    <row r="875" ht="13.5" customHeight="1"/>
+    <row r="876" ht="13.5" customHeight="1"/>
+    <row r="877" ht="13.5" customHeight="1"/>
+    <row r="878" ht="13.5" customHeight="1"/>
+    <row r="879" ht="13.5" customHeight="1"/>
+    <row r="880" ht="13.5" customHeight="1"/>
+    <row r="881" ht="13.5" customHeight="1"/>
+    <row r="882" ht="13.5" customHeight="1"/>
+    <row r="883" ht="13.5" customHeight="1"/>
+    <row r="884" ht="13.5" customHeight="1"/>
+    <row r="885" ht="13.5" customHeight="1"/>
+    <row r="886" ht="13.5" customHeight="1"/>
+    <row r="887" ht="13.5" customHeight="1"/>
+    <row r="888" ht="13.5" customHeight="1"/>
+    <row r="889" ht="13.5" customHeight="1"/>
+    <row r="890" ht="13.5" customHeight="1"/>
+    <row r="891" ht="13.5" customHeight="1"/>
+    <row r="892" ht="13.5" customHeight="1"/>
+    <row r="893" ht="13.5" customHeight="1"/>
+    <row r="894" ht="13.5" customHeight="1"/>
+    <row r="895" ht="13.5" customHeight="1"/>
+    <row r="896" ht="13.5" customHeight="1"/>
+    <row r="897" ht="13.5" customHeight="1"/>
+    <row r="898" ht="13.5" customHeight="1"/>
+    <row r="899" ht="13.5" customHeight="1"/>
+    <row r="900" ht="13.5" customHeight="1"/>
+    <row r="901" ht="13.5" customHeight="1"/>
+    <row r="902" ht="13.5" customHeight="1"/>
+    <row r="903" ht="13.5" customHeight="1"/>
+    <row r="904" ht="13.5" customHeight="1"/>
+    <row r="905" ht="13.5" customHeight="1"/>
+    <row r="906" ht="13.5" customHeight="1"/>
+    <row r="907" ht="13.5" customHeight="1"/>
+    <row r="908" ht="13.5" customHeight="1"/>
+    <row r="909" ht="13.5" customHeight="1"/>
+    <row r="910" ht="13.5" customHeight="1"/>
+    <row r="911" ht="13.5" customHeight="1"/>
+    <row r="912" ht="13.5" customHeight="1"/>
+    <row r="913" ht="13.5" customHeight="1"/>
+    <row r="914" ht="13.5" customHeight="1"/>
+    <row r="915" ht="13.5" customHeight="1"/>
+    <row r="916" ht="13.5" customHeight="1"/>
+    <row r="917" ht="13.5" customHeight="1"/>
+    <row r="918" ht="13.5" customHeight="1"/>
+    <row r="919" ht="13.5" customHeight="1"/>
+    <row r="920" ht="13.5" customHeight="1"/>
+    <row r="921" ht="13.5" customHeight="1"/>
+    <row r="922" ht="13.5" customHeight="1"/>
+    <row r="923" ht="13.5" customHeight="1"/>
+    <row r="924" ht="13.5" customHeight="1"/>
+    <row r="925" ht="13.5" customHeight="1"/>
+    <row r="926" ht="13.5" customHeight="1"/>
+    <row r="927" ht="13.5" customHeight="1"/>
+    <row r="928" ht="13.5" customHeight="1"/>
+    <row r="929" ht="13.5" customHeight="1"/>
+    <row r="930" ht="13.5" customHeight="1"/>
+    <row r="931" ht="13.5" customHeight="1"/>
+    <row r="932" ht="13.5" customHeight="1"/>
+    <row r="933" ht="13.5" customHeight="1"/>
+    <row r="934" ht="13.5" customHeight="1"/>
+    <row r="935" ht="13.5" customHeight="1"/>
+    <row r="936" ht="13.5" customHeight="1"/>
+    <row r="937" ht="13.5" customHeight="1"/>
+    <row r="938" ht="13.5" customHeight="1"/>
+    <row r="939" ht="13.5" customHeight="1"/>
+    <row r="940" ht="13.5" customHeight="1"/>
+    <row r="941" ht="13.5" customHeight="1"/>
+    <row r="942" ht="13.5" customHeight="1"/>
+    <row r="943" ht="13.5" customHeight="1"/>
+    <row r="944" ht="13.5" customHeight="1"/>
+    <row r="945" ht="13.5" customHeight="1"/>
+    <row r="946" ht="13.5" customHeight="1"/>
+    <row r="947" ht="13.5" customHeight="1"/>
+    <row r="948" ht="13.5" customHeight="1"/>
+    <row r="949" ht="13.5" customHeight="1"/>
+    <row r="950" ht="13.5" customHeight="1"/>
+    <row r="951" ht="13.5" customHeight="1"/>
+    <row r="952" ht="13.5" customHeight="1"/>
+    <row r="953" ht="13.5" customHeight="1"/>
+    <row r="954" ht="13.5" customHeight="1"/>
+    <row r="955" ht="13.5" customHeight="1"/>
+    <row r="956" ht="13.5" customHeight="1"/>
+    <row r="957" ht="13.5" customHeight="1"/>
+    <row r="958" ht="13.5" customHeight="1"/>
+    <row r="959" ht="13.5" customHeight="1"/>
+    <row r="960" ht="13.5" customHeight="1"/>
+    <row r="961" ht="13.5" customHeight="1"/>
+    <row r="962" ht="13.5" customHeight="1"/>
+    <row r="963" ht="13.5" customHeight="1"/>
+    <row r="964" ht="13.5" customHeight="1"/>
+    <row r="965" ht="13.5" customHeight="1"/>
+    <row r="966" ht="13.5" customHeight="1"/>
+    <row r="967" ht="13.5" customHeight="1"/>
+    <row r="968" ht="13.5" customHeight="1"/>
+    <row r="969" ht="13.5" customHeight="1"/>
+    <row r="970" ht="13.5" customHeight="1"/>
+    <row r="971" ht="13.5" customHeight="1"/>
+    <row r="972" ht="13.5" customHeight="1"/>
+    <row r="973" ht="13.5" customHeight="1"/>
+    <row r="974" ht="13.5" customHeight="1"/>
+    <row r="975" ht="13.5" customHeight="1"/>
+    <row r="976" ht="13.5" customHeight="1"/>
+    <row r="977" ht="13.5" customHeight="1"/>
+    <row r="978" ht="13.5" customHeight="1"/>
+    <row r="979" ht="13.5" customHeight="1"/>
+    <row r="980" ht="13.5" customHeight="1"/>
+    <row r="981" ht="13.5" customHeight="1"/>
+    <row r="982" ht="13.5" customHeight="1"/>
+    <row r="983" ht="13.5" customHeight="1"/>
+    <row r="984" ht="13.5" customHeight="1"/>
+    <row r="985" ht="13.5" customHeight="1"/>
+    <row r="986" ht="13.5" customHeight="1"/>
+    <row r="987" ht="13.5" customHeight="1"/>
+    <row r="988" ht="13.5" customHeight="1"/>
+    <row r="989" ht="13.5" customHeight="1"/>
+    <row r="990" ht="13.5" customHeight="1"/>
+    <row r="991" ht="13.5" customHeight="1"/>
+    <row r="992" ht="13.5" customHeight="1"/>
+    <row r="993" ht="13.5" customHeight="1"/>
+    <row r="994" ht="13.5" customHeight="1"/>
+    <row r="995" ht="13.5" customHeight="1"/>
+    <row r="996" ht="13.5" customHeight="1"/>
+    <row r="997" ht="13.5" customHeight="1"/>
+    <row r="998" ht="13.5" customHeight="1"/>
+    <row r="999" ht="13.5" customHeight="1"/>
+    <row r="1000" ht="13.5" customHeight="1"/>
   </sheetData>
   <mergeCells count="65">
-    <mergeCell ref="V57:X57"/>
-    <mergeCell ref="V58:X58"/>
-    <mergeCell ref="O59:X59"/>
-    <mergeCell ref="C51:H51"/>
-    <mergeCell ref="C52:H52"/>
-    <mergeCell ref="K52:P52"/>
-    <mergeCell ref="R52:X52"/>
-    <mergeCell ref="B53:H53"/>
-    <mergeCell ref="J53:P53"/>
-    <mergeCell ref="R53:X53"/>
-    <mergeCell ref="B38:H38"/>
-    <mergeCell ref="J38:P38"/>
-    <mergeCell ref="R38:X38"/>
-    <mergeCell ref="K39:P39"/>
-    <mergeCell ref="R39:X39"/>
+    <mergeCell ref="C40:H40"/>
+    <mergeCell ref="K40:P40"/>
+    <mergeCell ref="B41:H41"/>
+    <mergeCell ref="J41:P41"/>
+    <mergeCell ref="S41:X41"/>
+    <mergeCell ref="B43:F43"/>
+    <mergeCell ref="J43:N43"/>
+    <mergeCell ref="R43:V43"/>
+    <mergeCell ref="B50:H50"/>
+    <mergeCell ref="J50:P50"/>
+    <mergeCell ref="R50:X50"/>
+    <mergeCell ref="J17:N17"/>
+    <mergeCell ref="R17:V17"/>
+    <mergeCell ref="R12:X12"/>
+    <mergeCell ref="R13:X13"/>
+    <mergeCell ref="J25:P25"/>
+    <mergeCell ref="R25:X25"/>
+    <mergeCell ref="K12:P12"/>
+    <mergeCell ref="K13:P13"/>
+    <mergeCell ref="K14:P14"/>
+    <mergeCell ref="K15:P15"/>
+    <mergeCell ref="R15:X15"/>
+    <mergeCell ref="C2:X2"/>
+    <mergeCell ref="B4:F4"/>
+    <mergeCell ref="J4:N4"/>
+    <mergeCell ref="R4:V4"/>
+    <mergeCell ref="B11:H11"/>
+    <mergeCell ref="R11:X11"/>
+    <mergeCell ref="J11:P11"/>
+    <mergeCell ref="C12:H12"/>
+    <mergeCell ref="C13:H13"/>
+    <mergeCell ref="C14:H14"/>
+    <mergeCell ref="B15:H15"/>
+    <mergeCell ref="B17:F17"/>
     <mergeCell ref="J30:N30"/>
     <mergeCell ref="R30:V30"/>
     <mergeCell ref="B25:H25"/>
@@ -5241,45 +5278,26 @@
     <mergeCell ref="R28:X28"/>
     <mergeCell ref="C28:H28"/>
     <mergeCell ref="B30:F30"/>
-    <mergeCell ref="C12:H12"/>
-    <mergeCell ref="C13:H13"/>
-    <mergeCell ref="C14:H14"/>
-    <mergeCell ref="B15:H15"/>
-    <mergeCell ref="B17:F17"/>
-    <mergeCell ref="C2:X2"/>
-    <mergeCell ref="B4:F4"/>
-    <mergeCell ref="J4:N4"/>
-    <mergeCell ref="R4:V4"/>
-    <mergeCell ref="B11:H11"/>
-    <mergeCell ref="R11:X11"/>
+    <mergeCell ref="J27:P27"/>
+    <mergeCell ref="K28:P28"/>
+    <mergeCell ref="B38:H38"/>
+    <mergeCell ref="J38:P38"/>
+    <mergeCell ref="R38:X38"/>
+    <mergeCell ref="K39:P39"/>
+    <mergeCell ref="R39:X39"/>
+    <mergeCell ref="C39:H39"/>
+    <mergeCell ref="V57:X57"/>
+    <mergeCell ref="V58:X58"/>
+    <mergeCell ref="O59:X59"/>
+    <mergeCell ref="C51:H51"/>
+    <mergeCell ref="C52:H52"/>
+    <mergeCell ref="K52:P52"/>
+    <mergeCell ref="R52:X52"/>
+    <mergeCell ref="B53:H53"/>
+    <mergeCell ref="J53:P53"/>
+    <mergeCell ref="R53:X53"/>
     <mergeCell ref="K51:P51"/>
     <mergeCell ref="S51:X51"/>
-    <mergeCell ref="J11:P11"/>
-    <mergeCell ref="K12:P12"/>
-    <mergeCell ref="K13:P13"/>
-    <mergeCell ref="K14:P14"/>
-    <mergeCell ref="K15:P15"/>
-    <mergeCell ref="R15:X15"/>
-    <mergeCell ref="J17:N17"/>
-    <mergeCell ref="R17:V17"/>
-    <mergeCell ref="R12:X12"/>
-    <mergeCell ref="R13:X13"/>
-    <mergeCell ref="J25:P25"/>
-    <mergeCell ref="R25:X25"/>
-    <mergeCell ref="J27:P27"/>
-    <mergeCell ref="K28:P28"/>
-    <mergeCell ref="S41:X41"/>
-    <mergeCell ref="B43:F43"/>
-    <mergeCell ref="J43:N43"/>
-    <mergeCell ref="R43:V43"/>
-    <mergeCell ref="B50:H50"/>
-    <mergeCell ref="J50:P50"/>
-    <mergeCell ref="R50:X50"/>
-    <mergeCell ref="C39:H39"/>
-    <mergeCell ref="C40:H40"/>
-    <mergeCell ref="K40:P40"/>
-    <mergeCell ref="B41:H41"/>
-    <mergeCell ref="J41:P41"/>
   </mergeCells>
   <phoneticPr fontId="10"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>

</xml_diff>